<commit_message>
Changed year on application
</commit_message>
<xml_diff>
--- a/docs/Reference.xlsx
+++ b/docs/Reference.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18023"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3256671B-1BB0-46E8-BC27-DA4B93B7D725}" xr6:coauthVersionLast="17" xr6:coauthVersionMax="17" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="450" yWindow="705" windowWidth="13395" windowHeight="7455" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="450" yWindow="705" windowWidth="13395" windowHeight="7455" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Reference" sheetId="1" r:id="rId1"/>
@@ -13,12 +12,12 @@
     <sheet name="matchScore2016" sheetId="4" r:id="rId3"/>
     <sheet name="Score_2017" sheetId="5" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="171026"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="507" uniqueCount="404">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="378">
   <si>
     <t>Button Id</t>
   </si>
@@ -71,12 +70,6 @@
     <t>$auto_reach</t>
   </si>
   <si>
-    <t>auto_reach_defense</t>
-  </si>
-  <si>
-    <t>tinyint(1)</t>
-  </si>
-  <si>
     <t>auto_cross_btn</t>
   </si>
   <si>
@@ -152,9 +145,6 @@
     <t>$cross_def2</t>
   </si>
   <si>
-    <t>cross_defense2</t>
-  </si>
-  <si>
     <t>cross_def3_btn</t>
   </si>
   <si>
@@ -170,9 +160,6 @@
     <t>$cross_def3</t>
   </si>
   <si>
-    <t>cross_defense3</t>
-  </si>
-  <si>
     <t>cross_def4_btn</t>
   </si>
   <si>
@@ -188,9 +175,6 @@
     <t>$cross_def4</t>
   </si>
   <si>
-    <t>cross_defense4</t>
-  </si>
-  <si>
     <t>cross_def5_btn</t>
   </si>
   <si>
@@ -206,9 +190,6 @@
     <t>$cross_def5</t>
   </si>
   <si>
-    <t>cross_defense5</t>
-  </si>
-  <si>
     <t>open_def2_btn</t>
   </si>
   <si>
@@ -224,9 +205,6 @@
     <t>$open_def2</t>
   </si>
   <si>
-    <t>open_defense2</t>
-  </si>
-  <si>
     <t>open_def3_btn</t>
   </si>
   <si>
@@ -242,9 +220,6 @@
     <t>$open_def3</t>
   </si>
   <si>
-    <t>open_defense3</t>
-  </si>
-  <si>
     <t>open_def4_btn</t>
   </si>
   <si>
@@ -260,9 +235,6 @@
     <t>$open_def4</t>
   </si>
   <si>
-    <t>open_defense4</t>
-  </si>
-  <si>
     <t>open_def5_btn</t>
   </si>
   <si>
@@ -278,9 +250,6 @@
     <t>$open_def5</t>
   </si>
   <si>
-    <t>open_defense5</t>
-  </si>
-  <si>
     <t>pick_ball_btn</t>
   </si>
   <si>
@@ -296,9 +265,6 @@
     <t>$pick_ball</t>
   </si>
   <si>
-    <t>pick_boulder</t>
-  </si>
-  <si>
     <t>pass_ball_btn</t>
   </si>
   <si>
@@ -314,120 +280,27 @@
     <t>$pass_ball</t>
   </si>
   <si>
-    <t>pass_boulder</t>
-  </si>
-  <si>
-    <t>score_low_btn</t>
-  </si>
-  <si>
     <t>score_low</t>
   </si>
   <si>
-    <t>Score Low</t>
-  </si>
-  <si>
-    <t>score_low_badge</t>
-  </si>
-  <si>
-    <t>$score_low</t>
-  </si>
-  <si>
-    <t>score_high_btn</t>
-  </si>
-  <si>
     <t>score_high</t>
   </si>
   <si>
-    <t>Score High</t>
-  </si>
-  <si>
-    <t>score_high_badge</t>
-  </si>
-  <si>
-    <t>$score_high</t>
-  </si>
-  <si>
-    <t>reach_twr_btn</t>
-  </si>
-  <si>
-    <t>reach_twr</t>
-  </si>
-  <si>
-    <t>Reach Twr</t>
-  </si>
-  <si>
-    <t>reach_twr_badge</t>
-  </si>
-  <si>
-    <t>$reach_twr</t>
-  </si>
-  <si>
-    <t>get_on_tower</t>
-  </si>
-  <si>
-    <t>climb_twr_btn</t>
-  </si>
-  <si>
-    <t>climb_twr</t>
-  </si>
-  <si>
-    <t>Climb Twr</t>
-  </si>
-  <si>
-    <t>climb_twr_badge</t>
-  </si>
-  <si>
-    <t>$climb_twr</t>
-  </si>
-  <si>
-    <t>climb_tower</t>
-  </si>
-  <si>
-    <t>defense_btn</t>
-  </si>
-  <si>
     <t>defense</t>
   </si>
   <si>
     <t>Defense</t>
   </si>
   <si>
-    <t>defense_badge</t>
-  </si>
-  <si>
-    <t>$defense</t>
-  </si>
-  <si>
-    <t>fouls_btn</t>
-  </si>
-  <si>
     <t>fouls</t>
   </si>
   <si>
-    <t>Fouls</t>
-  </si>
-  <si>
-    <t>fouls_badge</t>
-  </si>
-  <si>
-    <t>$fouls</t>
-  </si>
-  <si>
-    <t>died_btn</t>
-  </si>
-  <si>
     <t>died</t>
   </si>
   <si>
     <t>Died</t>
   </si>
   <si>
-    <t>died_badge</t>
-  </si>
-  <si>
-    <t>$died</t>
-  </si>
-  <si>
     <t>red_def2</t>
   </si>
   <si>
@@ -1230,12 +1103,60 @@
   </si>
   <si>
     <t>Total points earned by the alliance in the Match</t>
+  </si>
+  <si>
+    <t>NYLI</t>
+  </si>
+  <si>
+    <t>auto_cross_line</t>
+  </si>
+  <si>
+    <t>auto_gear_left</t>
+  </si>
+  <si>
+    <t>auto_gear_center</t>
+  </si>
+  <si>
+    <t>tinyint(3)</t>
+  </si>
+  <si>
+    <t>auto_gear_right</t>
+  </si>
+  <si>
+    <t>auto_fuel_low</t>
+  </si>
+  <si>
+    <t>auto_fuel_high</t>
+  </si>
+  <si>
+    <t>telop_gears</t>
+  </si>
+  <si>
+    <t>teleop_fuel_low</t>
+  </si>
+  <si>
+    <t>teleop_fuel_high</t>
+  </si>
+  <si>
+    <t>teleop_climb</t>
+  </si>
+  <si>
+    <t>floor_gear_pickup</t>
+  </si>
+  <si>
+    <t>floor_ball_pickup</t>
+  </si>
+  <si>
+    <t>load_from_hopper</t>
+  </si>
+  <si>
+    <t>tech_fouls</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4">
     <font>
       <sz val="11"/>
@@ -1263,7 +1184,7 @@
       <name val="Source Code Pro"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1285,6 +1206,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFD8D8D8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1331,7 +1258,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" readingOrder="1"/>
@@ -1342,6 +1268,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1371,7 +1298,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -1430,7 +1357,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1463,26 +1390,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1515,23 +1425,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1707,11 +1600,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G34"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G31"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
-      <selection activeCell="B36" sqref="B36"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A18" sqref="A18:XFD18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1749,588 +1642,467 @@
       </c>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="11" t="s">
         <v>11</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>8</v>
+        <v>363</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>12</v>
+        <v>366</v>
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2" t="s">
+      <c r="D3" s="11"/>
+      <c r="E3" s="11" t="s">
         <v>16</v>
       </c>
       <c r="F3" s="2" t="s">
+        <v>364</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="B4" s="11" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4" s="2" t="s">
+      <c r="C4" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="D4" s="11"/>
+      <c r="E4" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2" t="s">
+      <c r="F4" s="2" t="s">
+        <v>365</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="B5" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="G4" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5" s="2" t="s">
+      <c r="C5" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="D5" s="11"/>
+      <c r="E5" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2" t="s">
+      <c r="F5" s="2" t="s">
+        <v>367</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="B6" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="G5" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="A6" s="2" t="s">
+      <c r="C6" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="D6" s="11"/>
+      <c r="E6" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2" t="s">
+      <c r="F6" s="2" t="s">
+        <v>368</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="11"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="2" t="s">
+        <v>369</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="11"/>
+      <c r="B8" s="11"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="B9" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="G6" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="A7" s="2" t="s">
+      <c r="C9" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="D9" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="E9" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="D7" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="A8" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="A9" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>49</v>
-      </c>
       <c r="F9" s="2" t="s">
-        <v>50</v>
+        <v>370</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:7">
-      <c r="A10" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>55</v>
+      <c r="A10" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>41</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>56</v>
+        <v>371</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:7">
-      <c r="A11" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>61</v>
+      <c r="A11" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>46</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>62</v>
+        <v>372</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:7">
-      <c r="A12" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>67</v>
+      <c r="A12" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>51</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>68</v>
+        <v>373</v>
       </c>
       <c r="G12" s="2" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:7">
-      <c r="A13" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>12</v>
-      </c>
+      <c r="A13" s="11"/>
+      <c r="B13" s="11"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
     </row>
     <row r="14" spans="1:7">
-      <c r="A14" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>79</v>
+      <c r="A14" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="E14" s="11" t="s">
+        <v>56</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>80</v>
+        <v>374</v>
       </c>
       <c r="G14" s="2" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:7">
-      <c r="A15" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>85</v>
+      <c r="A15" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="E15" s="11" t="s">
+        <v>61</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>86</v>
+        <v>375</v>
       </c>
       <c r="G15" s="2" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="16" spans="1:7">
-      <c r="A16" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="C16" s="3" t="s">
+      <c r="A16" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="E16" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="F16" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="D16" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="G16" s="3" t="s">
+      <c r="G16" s="2" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="17" spans="1:7">
-      <c r="A17" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>97</v>
+      <c r="A17" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="E17" s="11" t="s">
+        <v>71</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>98</v>
+        <v>376</v>
       </c>
       <c r="G17" s="2" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="18" spans="1:7">
-      <c r="A18" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="G18" s="2" t="s">
-        <v>12</v>
-      </c>
+      <c r="A18" s="11"/>
+      <c r="B18" s="11"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
     </row>
     <row r="19" spans="1:7">
-      <c r="A19" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>108</v>
+      <c r="A19" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="B19" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="D19" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="E19" s="11" t="s">
+        <v>76</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>105</v>
+        <v>91</v>
       </c>
       <c r="G19" s="2" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="20" spans="1:7">
-      <c r="A20" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="G20" s="2" t="s">
+      <c r="A20" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="B20" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="D20" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="E20" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>377</v>
+      </c>
+      <c r="G20" s="5" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="21" spans="1:7">
-      <c r="A21" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>119</v>
+      <c r="A21" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="C21" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="D21" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="E21" s="11" t="s">
+        <v>86</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>120</v>
+        <v>92</v>
       </c>
       <c r="G21" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="22" spans="1:7">
-      <c r="A22" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="G22" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7">
-      <c r="A23" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="G23" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
     <row r="24" spans="1:7">
-      <c r="A24" s="6" t="s">
-        <v>131</v>
-      </c>
-      <c r="B24" s="6" t="s">
-        <v>132</v>
-      </c>
-      <c r="C24" s="6" t="s">
-        <v>133</v>
-      </c>
-      <c r="D24" s="6" t="s">
-        <v>134</v>
-      </c>
-      <c r="E24" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="F24" s="6" t="s">
-        <v>132</v>
-      </c>
-      <c r="G24" s="6" t="s">
-        <v>12</v>
+      <c r="A24" t="s">
+        <v>94</v>
+      </c>
+      <c r="B24" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25" t="s">
+        <v>95</v>
+      </c>
+      <c r="B25" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="A26" t="s">
+        <v>96</v>
+      </c>
+      <c r="B26" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="27" spans="1:7">
       <c r="A27" t="s">
-        <v>136</v>
+        <v>97</v>
       </c>
       <c r="B27" t="s">
-        <v>136</v>
+        <v>97</v>
       </c>
     </row>
     <row r="28" spans="1:7">
       <c r="A28" t="s">
-        <v>137</v>
+        <v>98</v>
       </c>
       <c r="B28" t="s">
-        <v>137</v>
+        <v>98</v>
       </c>
     </row>
     <row r="29" spans="1:7">
       <c r="A29" t="s">
-        <v>138</v>
+        <v>99</v>
       </c>
       <c r="B29" t="s">
-        <v>138</v>
+        <v>99</v>
       </c>
     </row>
     <row r="30" spans="1:7">
       <c r="A30" t="s">
-        <v>139</v>
+        <v>100</v>
       </c>
       <c r="B30" t="s">
-        <v>139</v>
+        <v>100</v>
       </c>
     </row>
     <row r="31" spans="1:7">
       <c r="A31" t="s">
-        <v>140</v>
+        <v>101</v>
       </c>
       <c r="B31" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7">
-      <c r="A32" t="s">
-        <v>141</v>
-      </c>
-      <c r="B32" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2">
-      <c r="A33" t="s">
-        <v>142</v>
-      </c>
-      <c r="B33" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2">
-      <c r="A34" t="s">
-        <v>143</v>
-      </c>
-      <c r="B34" t="s">
-        <v>143</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -2340,10 +2112,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView workbookViewId="0" xr3:uid="{958C4451-9541-5A59-BF78-D2F731DF1C81}">
+    <sheetView workbookViewId="0">
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
@@ -2354,217 +2126,217 @@
     <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="8"/>
+    <col min="6" max="6" width="9.140625" style="7"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
-        <v>144</v>
+        <v>102</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>145</v>
+        <v>103</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>146</v>
+        <v>104</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>147</v>
+        <v>105</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="F1" s="8" t="s">
-        <v>149</v>
+        <v>106</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="2" t="s">
-        <v>150</v>
+        <v>108</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>151</v>
+        <v>109</v>
       </c>
       <c r="C2" s="2">
         <f>LEN(B2)</f>
         <v>10</v>
       </c>
-      <c r="D2" s="7" t="s">
-        <v>152</v>
+      <c r="D2" s="6" t="s">
+        <v>110</v>
       </c>
       <c r="E2" s="2">
         <f>LEN(D2)</f>
         <v>12</v>
       </c>
-      <c r="F2" s="8" t="s">
-        <v>153</v>
+      <c r="F2" s="7" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="2" t="s">
-        <v>150</v>
+        <v>108</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>154</v>
+        <v>112</v>
       </c>
       <c r="C3" s="2">
         <f t="shared" ref="C3:E9" si="0">LEN(B3)</f>
         <v>6</v>
       </c>
-      <c r="D3" s="7" t="s">
-        <v>155</v>
+      <c r="D3" s="6" t="s">
+        <v>113</v>
       </c>
       <c r="E3" s="2">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="F3" s="8" t="s">
-        <v>156</v>
+      <c r="F3" s="7" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="2" t="s">
-        <v>157</v>
+        <v>115</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>158</v>
+        <v>116</v>
       </c>
       <c r="C4" s="2">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="D4" s="7" t="s">
-        <v>159</v>
+      <c r="D4" s="6" t="s">
+        <v>117</v>
       </c>
       <c r="E4" s="2">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="F4" s="8" t="s">
-        <v>160</v>
+      <c r="F4" s="7" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="2" t="s">
-        <v>157</v>
+        <v>115</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>161</v>
+        <v>119</v>
       </c>
       <c r="C5" s="2">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="D5" s="7" t="s">
-        <v>162</v>
+      <c r="D5" s="6" t="s">
+        <v>120</v>
       </c>
       <c r="E5" s="2">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="F5" s="8" t="s">
-        <v>163</v>
+      <c r="F5" s="7" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="2" t="s">
-        <v>164</v>
+        <v>122</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>165</v>
+        <v>123</v>
       </c>
       <c r="C6" s="2">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="D6" s="7" t="s">
-        <v>166</v>
+      <c r="D6" s="6" t="s">
+        <v>124</v>
       </c>
       <c r="E6" s="2">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="F6" s="8" t="s">
-        <v>167</v>
+      <c r="F6" s="7" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="2" t="s">
-        <v>164</v>
+        <v>122</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>168</v>
+        <v>126</v>
       </c>
       <c r="C7" s="2">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="D7" s="7" t="s">
-        <v>169</v>
+      <c r="D7" s="6" t="s">
+        <v>127</v>
       </c>
       <c r="E7" s="2">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="F7" s="8" t="s">
-        <v>170</v>
+      <c r="F7" s="7" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="2" t="s">
-        <v>171</v>
+        <v>129</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>172</v>
+        <v>130</v>
       </c>
       <c r="C8" s="2">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="D8" s="7" t="s">
-        <v>173</v>
+      <c r="D8" s="6" t="s">
+        <v>131</v>
       </c>
       <c r="E8" s="2">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="F8" s="8" t="s">
-        <v>174</v>
+      <c r="F8" s="7" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="2" t="s">
-        <v>171</v>
+        <v>129</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>175</v>
+        <v>133</v>
       </c>
       <c r="C9" s="2">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="D9" s="7" t="s">
-        <v>176</v>
+      <c r="D9" s="6" t="s">
+        <v>134</v>
       </c>
       <c r="E9" s="2">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="F9" s="8" t="s">
-        <v>177</v>
+      <c r="F9" s="7" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="B10" t="s">
-        <v>178</v>
-      </c>
-      <c r="C10" s="10">
+        <v>136</v>
+      </c>
+      <c r="C10" s="9">
         <f>MAX(C2:C9)</f>
         <v>13</v>
       </c>
-      <c r="D10" s="9" t="s">
-        <v>178</v>
-      </c>
-      <c r="E10" s="10">
+      <c r="D10" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="E10" s="9">
         <f>MAX(E2:E9)</f>
         <v>15</v>
       </c>
@@ -2576,807 +2348,807 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J93"/>
   <sheetViews>
-    <sheetView workbookViewId="0" xr3:uid="{842E5F09-E766-5B8D-85AF-A39847EA96FD}">
+    <sheetView workbookViewId="0">
       <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="6" width="9.140625" style="4"/>
-    <col min="7" max="7" width="23.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.85546875" style="4" customWidth="1"/>
-    <col min="9" max="9" width="25.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="26.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="4"/>
+    <col min="1" max="6" width="9.140625" style="3"/>
+    <col min="7" max="7" width="23.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.85546875" style="3" customWidth="1"/>
+    <col min="9" max="9" width="25.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="26.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" s="4" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" s="4" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" s="4" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" s="4" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" s="4" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" s="4" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" s="4" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" s="4" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="A11" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="A12" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="J12" s="3" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="A13" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="I13" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="J13" s="3" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="A14" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I14" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="J14" s="3" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
+      <c r="A15" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
+      <c r="A16" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
+      <c r="A17" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="I17" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="J17" s="3" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
+      <c r="A18" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="I18" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="J18" s="3" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
+      <c r="A19" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="I19" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="J19" s="3" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
-      <c r="A2" s="5" t="s">
+    <row r="20" spans="1:10">
+      <c r="A20" s="4" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="3" spans="1:10">
-      <c r="A3" s="5" t="s">
+      <c r="G20" s="3" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
-      <c r="A4" s="5" t="s">
+    <row r="21" spans="1:10">
+      <c r="A21" s="4" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="5" spans="1:10">
-      <c r="A5" s="5" t="s">
+      <c r="G21" s="3" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="6" spans="1:10">
-      <c r="A6" s="5" t="s">
+      <c r="H21" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="I21" s="3" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="7" spans="1:10">
-      <c r="A7" s="5" t="s">
+      <c r="J21" s="3" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
-      <c r="A8" s="5" t="s">
+    <row r="22" spans="1:10">
+      <c r="A22" s="4" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="9" spans="1:10">
-      <c r="A9" s="5" t="s">
+      <c r="G22" s="3" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="10" spans="1:10">
-      <c r="A10" s="5" t="s">
+      <c r="H22" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="I10" s="4" t="s">
+      <c r="I22" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="J22" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
+      <c r="A23" s="4" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="11" spans="1:10">
-      <c r="A11" s="5" t="s">
+      <c r="G23" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="G11" s="4" t="s">
+      <c r="H23" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="I23" s="3" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="12" spans="1:10">
-      <c r="A12" s="5" t="s">
+      <c r="J23" s="3" t="s">
         <v>192</v>
       </c>
-      <c r="G12" s="4" t="s">
+    </row>
+    <row r="24" spans="1:10">
+      <c r="A24" s="4" t="s">
         <v>193</v>
       </c>
-      <c r="H12" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="I12" s="4" t="s">
+      <c r="G24" s="3" t="s">
         <v>194</v>
       </c>
-      <c r="J12" s="4" t="s">
+      <c r="H24" s="3" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="13" spans="1:10">
-      <c r="A13" s="5" t="s">
+      <c r="I24" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="J24" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10">
+      <c r="A25" s="4" t="s">
         <v>196</v>
       </c>
-      <c r="G13" s="4" t="s">
+      <c r="G25" s="3" t="s">
         <v>197</v>
       </c>
-      <c r="H13" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="I13" s="4" t="s">
+      <c r="H25" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="I25" s="3" t="s">
         <v>198</v>
       </c>
-      <c r="J13" s="4" t="s">
+      <c r="J25" s="3" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
-      <c r="A14" s="5" t="s">
+    <row r="26" spans="1:10">
+      <c r="A26" s="4" t="s">
         <v>200</v>
       </c>
-      <c r="G14" s="4" t="s">
+      <c r="G26" s="3" t="s">
         <v>201</v>
       </c>
-      <c r="H14" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="I14" s="4" t="s">
+      <c r="H26" s="3" t="s">
         <v>202</v>
       </c>
-      <c r="J14" s="4" t="s">
+      <c r="I26" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="J26" s="3" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10">
+      <c r="A27" s="4" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="15" spans="1:10">
-      <c r="A15" s="5" t="s">
+      <c r="G27" s="3" t="s">
         <v>204</v>
       </c>
-      <c r="G15" s="4" t="s">
+      <c r="H27" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="I27" s="3" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="16" spans="1:10">
-      <c r="A16" s="5" t="s">
+      <c r="J27" s="3" t="s">
         <v>206</v>
       </c>
-      <c r="G16" s="4" t="s">
+    </row>
+    <row r="28" spans="1:10">
+      <c r="A28" s="4" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="17" spans="1:10">
-      <c r="A17" s="5" t="s">
+      <c r="G28" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="G17" s="4" t="s">
+      <c r="H28" s="3" t="s">
         <v>209</v>
       </c>
-      <c r="H17" s="4" t="s">
+      <c r="I28" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="J28" s="3" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10">
+      <c r="A29" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="I17" s="4" t="s">
+      <c r="G29" s="3" t="s">
         <v>211</v>
       </c>
-      <c r="J17" s="4" t="s">
+      <c r="H29" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="I29" s="3" t="s">
         <v>212</v>
       </c>
-    </row>
-    <row r="18" spans="1:10">
-      <c r="A18" s="5" t="s">
+      <c r="J29" s="3" t="s">
         <v>213</v>
       </c>
-      <c r="G18" s="4" t="s">
+    </row>
+    <row r="30" spans="1:10">
+      <c r="A30" s="4" t="s">
         <v>214</v>
       </c>
-      <c r="H18" s="4" t="s">
+      <c r="G30" s="3" t="s">
         <v>215</v>
       </c>
-      <c r="I18" s="4" t="s">
+      <c r="H30" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="J18" s="4" t="s">
+      <c r="I30" s="3" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="19" spans="1:10">
-      <c r="A19" s="5" t="s">
+      <c r="J30" s="3" t="s">
         <v>218</v>
       </c>
-      <c r="G19" s="4" t="s">
+    </row>
+    <row r="31" spans="1:10">
+      <c r="A31" s="4" t="s">
         <v>219</v>
       </c>
-      <c r="H19" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="I19" s="4" t="s">
+      <c r="G31" s="3" t="s">
         <v>220</v>
       </c>
-      <c r="J19" s="4" t="s">
+      <c r="H31" s="3" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="20" spans="1:10">
-      <c r="A20" s="5" t="s">
+      <c r="I31" s="3" t="s">
         <v>222</v>
       </c>
-      <c r="G20" s="4" t="s">
+      <c r="J31" s="3" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="21" spans="1:10">
-      <c r="A21" s="5" t="s">
+    <row r="32" spans="1:10">
+      <c r="A32" s="4" t="s">
         <v>224</v>
       </c>
-      <c r="G21" s="4" t="s">
+      <c r="G32" s="3" t="s">
         <v>225</v>
       </c>
-      <c r="H21" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="I21" s="4" t="s">
+      <c r="H32" s="3" t="s">
         <v>226</v>
       </c>
-      <c r="J21" s="4" t="s">
+      <c r="I32" s="3" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="22" spans="1:10">
-      <c r="A22" s="5" t="s">
+      <c r="J32" s="3" t="s">
         <v>228</v>
       </c>
-      <c r="G22" s="4" t="s">
+    </row>
+    <row r="33" spans="1:10">
+      <c r="A33" s="4" t="s">
         <v>229</v>
       </c>
-      <c r="H22" s="4" t="s">
+      <c r="G33" s="3" t="s">
         <v>230</v>
       </c>
-      <c r="I22" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="J22" s="4" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10">
-      <c r="A23" s="5" t="s">
+    </row>
+    <row r="34" spans="1:10">
+      <c r="A34" s="4" t="s">
         <v>231</v>
       </c>
-      <c r="G23" s="4" t="s">
+      <c r="G34" s="3" t="s">
         <v>232</v>
       </c>
-      <c r="H23" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="I23" s="4" t="s">
+    </row>
+    <row r="35" spans="1:10">
+      <c r="A35" s="4" t="s">
         <v>233</v>
       </c>
-      <c r="J23" s="4" t="s">
+      <c r="G35" s="3" t="s">
         <v>234</v>
       </c>
-    </row>
-    <row r="24" spans="1:10">
-      <c r="A24" s="5" t="s">
+      <c r="H35" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="I35" s="3" t="s">
         <v>235</v>
       </c>
-      <c r="G24" s="4" t="s">
+      <c r="J35" s="3" t="s">
         <v>236</v>
       </c>
-      <c r="H24" s="4" t="s">
+    </row>
+    <row r="36" spans="1:10">
+      <c r="A36" s="4" t="s">
         <v>237</v>
       </c>
-      <c r="I24" s="4" t="s">
-        <v>137</v>
-      </c>
-      <c r="J24" s="4" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10">
-      <c r="A25" s="5" t="s">
+      <c r="G36" s="3" t="s">
         <v>238</v>
       </c>
-      <c r="G25" s="4" t="s">
+      <c r="H36" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="I36" s="3" t="s">
         <v>239</v>
       </c>
-      <c r="H25" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="I25" s="4" t="s">
+      <c r="J36" s="3" t="s">
         <v>240</v>
       </c>
-      <c r="J25" s="4" t="s">
+    </row>
+    <row r="37" spans="1:10">
+      <c r="A37" s="4" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="26" spans="1:10">
-      <c r="A26" s="5" t="s">
+      <c r="G37" s="3" t="s">
         <v>242</v>
       </c>
-      <c r="G26" s="4" t="s">
+    </row>
+    <row r="38" spans="1:10">
+      <c r="A38" s="4" t="s">
         <v>243</v>
       </c>
-      <c r="H26" s="4" t="s">
+      <c r="G38" s="3" t="s">
         <v>244</v>
       </c>
-      <c r="I26" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="J26" s="4" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10">
-      <c r="A27" s="5" t="s">
+    </row>
+    <row r="39" spans="1:10">
+      <c r="A39" s="4" t="s">
         <v>245</v>
       </c>
-      <c r="G27" s="4" t="s">
+      <c r="G39" s="3" t="s">
         <v>246</v>
       </c>
-      <c r="H27" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="I27" s="4" t="s">
+    </row>
+    <row r="40" spans="1:10">
+      <c r="A40" s="4" t="s">
         <v>247</v>
       </c>
-      <c r="J27" s="4" t="s">
+      <c r="G40" s="3" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="28" spans="1:10">
-      <c r="A28" s="5" t="s">
+    <row r="41" spans="1:10">
+      <c r="A41" s="4" t="s">
         <v>249</v>
       </c>
-      <c r="G28" s="4" t="s">
+      <c r="G41" s="3" t="s">
         <v>250</v>
       </c>
-      <c r="H28" s="4" t="s">
+    </row>
+    <row r="42" spans="1:10">
+      <c r="A42" s="4" t="s">
         <v>251</v>
       </c>
-      <c r="I28" s="4" t="s">
-        <v>139</v>
-      </c>
-      <c r="J28" s="4" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10">
-      <c r="A29" s="5" t="s">
+      <c r="G42" s="3" t="s">
         <v>252</v>
       </c>
-      <c r="G29" s="4" t="s">
+    </row>
+    <row r="43" spans="1:10">
+      <c r="A43" s="4" t="s">
         <v>253</v>
       </c>
-      <c r="H29" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="I29" s="4" t="s">
+      <c r="G43" s="3" t="s">
         <v>254</v>
       </c>
-      <c r="J29" s="4" t="s">
+    </row>
+    <row r="44" spans="1:10">
+      <c r="A44" s="4" t="s">
         <v>255</v>
       </c>
-    </row>
-    <row r="30" spans="1:10">
-      <c r="A30" s="5" t="s">
+      <c r="G44" s="3" t="s">
         <v>256</v>
       </c>
-      <c r="G30" s="4" t="s">
+    </row>
+    <row r="45" spans="1:10">
+      <c r="A45" s="4" t="s">
         <v>257</v>
       </c>
-      <c r="H30" s="4" t="s">
+      <c r="G45" s="3" t="s">
         <v>258</v>
       </c>
-      <c r="I30" s="4" t="s">
+      <c r="H45" s="3" t="s">
         <v>259</v>
       </c>
-      <c r="J30" s="4" t="s">
+      <c r="I45" s="3" t="s">
         <v>260</v>
       </c>
-    </row>
-    <row r="31" spans="1:10">
-      <c r="A31" s="5" t="s">
+      <c r="J45" s="3" t="s">
         <v>261</v>
       </c>
-      <c r="G31" s="4" t="s">
+    </row>
+    <row r="46" spans="1:10">
+      <c r="A46" s="4" t="s">
         <v>262</v>
       </c>
-      <c r="H31" s="4" t="s">
+      <c r="G46" s="3" t="s">
         <v>263</v>
       </c>
-      <c r="I31" s="4" t="s">
+      <c r="H46" s="3" t="s">
         <v>264</v>
       </c>
-      <c r="J31" s="4" t="s">
+      <c r="I46" s="3" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="32" spans="1:10">
-      <c r="A32" s="5" t="s">
+      <c r="J46" s="3" t="s">
         <v>266</v>
       </c>
-      <c r="G32" s="4" t="s">
+    </row>
+    <row r="47" spans="1:10">
+      <c r="A47" s="4" t="s">
         <v>267</v>
       </c>
-      <c r="H32" s="4" t="s">
+      <c r="G47" s="3" t="s">
         <v>268</v>
       </c>
-      <c r="I32" s="4" t="s">
+      <c r="H47" s="3" t="s">
         <v>269</v>
       </c>
-      <c r="J32" s="4" t="s">
+      <c r="I47" s="3" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="33" spans="1:10">
-      <c r="A33" s="5" t="s">
+      <c r="J47" s="3" t="s">
         <v>271</v>
       </c>
-      <c r="G33" s="4" t="s">
+    </row>
+    <row r="48" spans="1:10">
+      <c r="A48" s="4" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="34" spans="1:10">
-      <c r="A34" s="5" t="s">
+    <row r="49" spans="1:1">
+      <c r="A49" s="4" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1">
+      <c r="A50" s="4" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1">
+      <c r="A51" s="4" t="s">
         <v>273</v>
       </c>
-      <c r="G34" s="4" t="s">
+    </row>
+    <row r="52" spans="1:1">
+      <c r="A52" s="4" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1">
+      <c r="A53" s="4" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1">
+      <c r="A54" s="4" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1">
+      <c r="A55" s="4" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1">
+      <c r="A56" s="4" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1">
+      <c r="A57" s="4" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1">
+      <c r="A58" s="4" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1">
+      <c r="A59" s="4" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1">
+      <c r="A60" s="4" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1">
+      <c r="A61" s="4" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1">
+      <c r="A62" s="4" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1">
+      <c r="A63" s="4" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="35" spans="1:10">
-      <c r="A35" s="5" t="s">
+    <row r="64" spans="1:1">
+      <c r="A64" s="4" t="s">
         <v>275</v>
       </c>
-      <c r="G35" s="4" t="s">
+    </row>
+    <row r="65" spans="1:1">
+      <c r="A65" s="4" t="s">
         <v>276</v>
       </c>
-      <c r="H35" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="I35" s="4" t="s">
+    </row>
+    <row r="66" spans="1:1">
+      <c r="A66" s="4" t="s">
         <v>277</v>
       </c>
-      <c r="J35" s="4" t="s">
+    </row>
+    <row r="67" spans="1:1">
+      <c r="A67" s="4" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="36" spans="1:10">
-      <c r="A36" s="5" t="s">
+    <row r="68" spans="1:1">
+      <c r="A68" s="4" t="s">
         <v>279</v>
       </c>
-      <c r="G36" s="4" t="s">
+    </row>
+    <row r="69" spans="1:1">
+      <c r="A69" s="4" t="s">
         <v>280</v>
       </c>
-      <c r="H36" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="I36" s="4" t="s">
+    </row>
+    <row r="70" spans="1:1">
+      <c r="A70" s="4" t="s">
         <v>281</v>
       </c>
-      <c r="J36" s="4" t="s">
+    </row>
+    <row r="71" spans="1:1">
+      <c r="A71" s="4" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1">
+      <c r="A72" s="4" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="37" spans="1:10">
-      <c r="A37" s="5" t="s">
+    <row r="73" spans="1:1">
+      <c r="A73" s="4" t="s">
         <v>283</v>
       </c>
-      <c r="G37" s="4" t="s">
+    </row>
+    <row r="74" spans="1:1">
+      <c r="A74" s="4" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1">
+      <c r="A75" s="4" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1">
+      <c r="A76" s="4" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1">
+      <c r="A77" s="4" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1">
+      <c r="A78" s="4" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1">
+      <c r="A79" s="4" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1">
+      <c r="A80" s="4" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="38" spans="1:10">
-      <c r="A38" s="5" t="s">
+    <row r="81" spans="1:1">
+      <c r="A81" s="4" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1">
+      <c r="A82" s="4" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1">
+      <c r="A83" s="4" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1">
+      <c r="A84" s="4" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1">
+      <c r="A85" s="4" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1">
+      <c r="A86" s="4" t="s">
         <v>285</v>
       </c>
-      <c r="G38" s="4" t="s">
+    </row>
+    <row r="87" spans="1:1">
+      <c r="A87" s="4" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="39" spans="1:10">
-      <c r="A39" s="5" t="s">
+    <row r="88" spans="1:1">
+      <c r="A88" s="4" t="s">
         <v>287</v>
       </c>
-      <c r="G39" s="4" t="s">
+    </row>
+    <row r="89" spans="1:1">
+      <c r="A89" s="4" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1">
+      <c r="A90" s="4" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="40" spans="1:10">
-      <c r="A40" s="5" t="s">
+    <row r="91" spans="1:1">
+      <c r="A91" s="4" t="s">
         <v>289</v>
       </c>
-      <c r="G40" s="4" t="s">
+    </row>
+    <row r="92" spans="1:1">
+      <c r="A92" s="4" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="41" spans="1:10">
-      <c r="A41" s="5" t="s">
+    <row r="93" spans="1:1">
+      <c r="A93" s="4" t="s">
         <v>291</v>
-      </c>
-      <c r="G41" s="4" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10">
-      <c r="A42" s="5" t="s">
-        <v>293</v>
-      </c>
-      <c r="G42" s="4" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10">
-      <c r="A43" s="5" t="s">
-        <v>295</v>
-      </c>
-      <c r="G43" s="4" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10">
-      <c r="A44" s="5" t="s">
-        <v>297</v>
-      </c>
-      <c r="G44" s="4" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10">
-      <c r="A45" s="5" t="s">
-        <v>299</v>
-      </c>
-      <c r="G45" s="4" t="s">
-        <v>300</v>
-      </c>
-      <c r="H45" s="4" t="s">
-        <v>301</v>
-      </c>
-      <c r="I45" s="4" t="s">
-        <v>302</v>
-      </c>
-      <c r="J45" s="4" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10">
-      <c r="A46" s="5" t="s">
-        <v>304</v>
-      </c>
-      <c r="G46" s="4" t="s">
-        <v>305</v>
-      </c>
-      <c r="H46" s="4" t="s">
-        <v>306</v>
-      </c>
-      <c r="I46" s="4" t="s">
-        <v>307</v>
-      </c>
-      <c r="J46" s="4" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10">
-      <c r="A47" s="5" t="s">
-        <v>309</v>
-      </c>
-      <c r="G47" s="4" t="s">
-        <v>310</v>
-      </c>
-      <c r="H47" s="4" t="s">
-        <v>311</v>
-      </c>
-      <c r="I47" s="4" t="s">
-        <v>312</v>
-      </c>
-      <c r="J47" s="4" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10">
-      <c r="A48" s="5" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1">
-      <c r="A49" s="5" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1">
-      <c r="A50" s="5" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="51" spans="1:1">
-      <c r="A51" s="5" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="52" spans="1:1">
-      <c r="A52" s="5" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="53" spans="1:1">
-      <c r="A53" s="5" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="54" spans="1:1">
-      <c r="A54" s="5" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="55" spans="1:1">
-      <c r="A55" s="5" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="56" spans="1:1">
-      <c r="A56" s="5" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="57" spans="1:1">
-      <c r="A57" s="5" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="58" spans="1:1">
-      <c r="A58" s="5" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="59" spans="1:1">
-      <c r="A59" s="5" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="60" spans="1:1">
-      <c r="A60" s="5" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="61" spans="1:1">
-      <c r="A61" s="5" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="62" spans="1:1">
-      <c r="A62" s="5" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="63" spans="1:1">
-      <c r="A63" s="5" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="64" spans="1:1">
-      <c r="A64" s="5" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="65" spans="1:1">
-      <c r="A65" s="5" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="66" spans="1:1">
-      <c r="A66" s="5" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="67" spans="1:1">
-      <c r="A67" s="5" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="68" spans="1:1">
-      <c r="A68" s="5" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="69" spans="1:1">
-      <c r="A69" s="5" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="70" spans="1:1">
-      <c r="A70" s="5" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="71" spans="1:1">
-      <c r="A71" s="5" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="72" spans="1:1">
-      <c r="A72" s="5" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="73" spans="1:1">
-      <c r="A73" s="5" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="74" spans="1:1">
-      <c r="A74" s="5" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="75" spans="1:1">
-      <c r="A75" s="5" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="76" spans="1:1">
-      <c r="A76" s="5" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="77" spans="1:1">
-      <c r="A77" s="5" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="78" spans="1:1">
-      <c r="A78" s="5" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="79" spans="1:1">
-      <c r="A79" s="5" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="80" spans="1:1">
-      <c r="A80" s="5" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="81" spans="1:1">
-      <c r="A81" s="5" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="82" spans="1:1">
-      <c r="A82" s="5" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="83" spans="1:1">
-      <c r="A83" s="5" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="84" spans="1:1">
-      <c r="A84" s="5" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="85" spans="1:1">
-      <c r="A85" s="5" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="86" spans="1:1">
-      <c r="A86" s="5" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="87" spans="1:1">
-      <c r="A87" s="5" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="88" spans="1:1">
-      <c r="A88" s="5" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="89" spans="1:1">
-      <c r="A89" s="5" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="90" spans="1:1">
-      <c r="A90" s="5" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="91" spans="1:1">
-      <c r="A91" s="5" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="92" spans="1:1">
-      <c r="A92" s="5" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="93" spans="1:1">
-      <c r="A93" s="5" t="s">
-        <v>333</v>
       </c>
     </row>
   </sheetData>
@@ -3386,11 +3158,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C8E7B48-9C32-4ABD-9EE1-B897ECE3B734}">
-  <dimension ref="A1:C39"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0" xr3:uid="{5DE94560-C6DC-585B-8028-05C0521D1817}">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3403,341 +3175,354 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>334</v>
+        <v>292</v>
       </c>
       <c r="B1" t="s">
-        <v>335</v>
+        <v>293</v>
+      </c>
+      <c r="C1" t="s">
+        <v>362</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>336</v>
+        <v>294</v>
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="11" t="s">
-        <v>337</v>
-      </c>
-      <c r="B4" s="11" t="s">
-        <v>338</v>
+      <c r="A4" s="10" t="s">
+        <v>295</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>296</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="2" t="s">
-        <v>339</v>
+        <v>297</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>340</v>
+        <v>298</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="2" t="s">
-        <v>257</v>
+        <v>215</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>341</v>
+        <v>299</v>
       </c>
       <c r="C6" t="s">
-        <v>342</v>
+        <v>300</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="2" t="s">
-        <v>262</v>
+        <v>220</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>343</v>
+        <v>301</v>
       </c>
       <c r="C7" t="s">
-        <v>344</v>
+        <v>302</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="2" t="s">
-        <v>267</v>
+        <v>225</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>345</v>
+        <v>303</v>
       </c>
       <c r="C8" t="s">
-        <v>346</v>
+        <v>304</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" t="s">
-        <v>347</v>
+        <v>305</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="2" t="s">
-        <v>348</v>
+        <v>306</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>349</v>
+        <v>307</v>
       </c>
       <c r="C10" t="s">
-        <v>350</v>
+        <v>308</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="2" t="s">
-        <v>351</v>
+        <v>309</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>349</v>
+        <v>307</v>
       </c>
       <c r="C11" t="s">
-        <v>352</v>
+        <v>310</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="2" t="s">
-        <v>353</v>
+        <v>311</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>354</v>
+        <v>312</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="2" t="s">
-        <v>355</v>
+        <v>313</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>354</v>
+        <v>312</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="2" t="s">
-        <v>356</v>
+        <v>314</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>357</v>
+        <v>315</v>
       </c>
       <c r="C14" t="s">
-        <v>358</v>
+        <v>316</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="2" t="s">
-        <v>359</v>
+        <v>317</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>357</v>
+        <v>315</v>
       </c>
       <c r="C15" t="s">
-        <v>360</v>
+        <v>318</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="2" t="s">
-        <v>361</v>
+        <v>319</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>357</v>
+        <v>315</v>
       </c>
       <c r="C16" t="s">
-        <v>362</v>
+        <v>320</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="2" t="s">
-        <v>363</v>
+        <v>321</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>357</v>
+        <v>315</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="2" t="s">
-        <v>364</v>
+        <v>322</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>349</v>
+        <v>307</v>
       </c>
       <c r="C18" t="s">
-        <v>365</v>
+        <v>323</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="2" t="s">
-        <v>366</v>
+        <v>324</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>349</v>
+        <v>307</v>
       </c>
       <c r="C19" t="s">
-        <v>367</v>
+        <v>325</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" s="2" t="s">
-        <v>368</v>
+        <v>326</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>369</v>
+        <v>327</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" s="2" t="s">
-        <v>370</v>
+        <v>328</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>371</v>
+        <v>329</v>
       </c>
       <c r="C21" t="s">
-        <v>372</v>
+        <v>330</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" s="2" t="s">
-        <v>373</v>
+        <v>331</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>374</v>
+        <v>332</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" s="2" t="s">
-        <v>375</v>
+        <v>333</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>376</v>
+        <v>334</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" s="2" t="s">
-        <v>377</v>
+        <v>335</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>376</v>
+        <v>334</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" s="2" t="s">
-        <v>219</v>
+        <v>177</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>378</v>
+        <v>336</v>
       </c>
       <c r="C25" t="s">
-        <v>379</v>
+        <v>337</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" s="2" t="s">
-        <v>272</v>
+        <v>230</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>380</v>
+        <v>338</v>
       </c>
       <c r="C26" t="s">
-        <v>381</v>
+        <v>339</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" s="2" t="s">
-        <v>205</v>
+        <v>163</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>382</v>
+        <v>340</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" s="2" t="s">
-        <v>383</v>
+        <v>341</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>384</v>
+        <v>342</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" s="2" t="s">
-        <v>385</v>
+        <v>343</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>386</v>
+        <v>344</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" s="2" t="s">
-        <v>387</v>
+        <v>345</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>388</v>
+        <v>346</v>
       </c>
     </row>
     <row r="31" spans="1:3">
       <c r="A31" s="2" t="s">
-        <v>290</v>
+        <v>248</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>389</v>
+        <v>347</v>
       </c>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" s="2" t="s">
-        <v>390</v>
+        <v>348</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>391</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
       <c r="A33" s="2" t="s">
-        <v>392</v>
+        <v>350</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>393</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
       <c r="A34" s="2" t="s">
-        <v>394</v>
+        <v>352</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
       <c r="A35" s="2" t="s">
-        <v>396</v>
+        <v>354</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
       <c r="A36" s="2" t="s">
-        <v>398</v>
+        <v>356</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
       <c r="A37" s="2" t="s">
-        <v>400</v>
+        <v>358</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
       <c r="A38" s="2" t="s">
-        <v>223</v>
+        <v>181</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
       <c r="A39" s="2" t="s">
-        <v>296</v>
+        <v>254</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>403</v>
+        <v>361</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="C40" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="C41" t="s">
+        <v>93</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed index.html to 2017
</commit_message>
<xml_diff>
--- a/docs/Reference.xlsx
+++ b/docs/Reference.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="450" yWindow="705" windowWidth="13395" windowHeight="7455" activeTab="3"/>
+    <workbookView xWindow="450" yWindow="705" windowWidth="13395" windowHeight="7455"/>
   </bookViews>
   <sheets>
     <sheet name="Reference" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="378">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="451" uniqueCount="372">
   <si>
     <t>Button Id</t>
   </si>
@@ -40,246 +40,36 @@
     <t>Data Type</t>
   </si>
   <si>
-    <t>auto_position_btn</t>
-  </si>
-  <si>
-    <t>auto_position</t>
-  </si>
-  <si>
-    <t>Position</t>
-  </si>
-  <si>
-    <t>auto_position_badge</t>
-  </si>
-  <si>
-    <t>$auto_position</t>
-  </si>
-  <si>
     <t>tinyint(4)</t>
   </si>
   <si>
-    <t>auto_reach_btn</t>
-  </si>
-  <si>
-    <t>auto_reach</t>
-  </si>
-  <si>
-    <t>Reach Defense</t>
-  </si>
-  <si>
-    <t>$auto_reach</t>
-  </si>
-  <si>
-    <t>auto_cross_btn</t>
-  </si>
-  <si>
-    <t>auto_cross</t>
-  </si>
-  <si>
-    <t>Cross Defense</t>
-  </si>
-  <si>
-    <t>$auto_cross</t>
-  </si>
-  <si>
     <t>auto_cross_defense</t>
   </si>
   <si>
-    <t>auto_low_btn</t>
-  </si>
-  <si>
-    <t>auto_low</t>
-  </si>
-  <si>
-    <t>Low Goal</t>
-  </si>
-  <si>
-    <t>$auto_low</t>
-  </si>
-  <si>
     <t>auto_low_goal</t>
   </si>
   <si>
-    <t>auto_high_btn</t>
-  </si>
-  <si>
-    <t>auto_high</t>
-  </si>
-  <si>
-    <t>High Goal</t>
-  </si>
-  <si>
-    <t>$auto_high</t>
-  </si>
-  <si>
     <t>auto_high_goal</t>
   </si>
   <si>
-    <t>cross_low_bar_btn</t>
-  </si>
-  <si>
     <t>cross_low_bar</t>
   </si>
   <si>
-    <t>Cross Low Bar</t>
-  </si>
-  <si>
-    <t>cross_low_bar_badge</t>
-  </si>
-  <si>
-    <t>$cross_low_bar</t>
-  </si>
-  <si>
-    <t>cross_def2_btn</t>
-  </si>
-  <si>
     <t>cross_def2</t>
   </si>
   <si>
-    <t>Cross Def 2</t>
-  </si>
-  <si>
-    <t>cross_def2_badge</t>
-  </si>
-  <si>
-    <t>$cross_def2</t>
-  </si>
-  <si>
-    <t>cross_def3_btn</t>
-  </si>
-  <si>
     <t>cross_def3</t>
   </si>
   <si>
-    <t>Cross Def 3</t>
-  </si>
-  <si>
-    <t>cross_def3_badge</t>
-  </si>
-  <si>
-    <t>$cross_def3</t>
-  </si>
-  <si>
-    <t>cross_def4_btn</t>
-  </si>
-  <si>
     <t>cross_def4</t>
   </si>
   <si>
-    <t>Cross Def 4</t>
-  </si>
-  <si>
-    <t>cross_def4_badge</t>
-  </si>
-  <si>
-    <t>$cross_def4</t>
-  </si>
-  <si>
-    <t>cross_def5_btn</t>
-  </si>
-  <si>
     <t>cross_def5</t>
   </si>
   <si>
-    <t>Cross Def 5</t>
-  </si>
-  <si>
-    <t>cross_def5_badge</t>
-  </si>
-  <si>
-    <t>$cross_def5</t>
-  </si>
-  <si>
-    <t>open_def2_btn</t>
-  </si>
-  <si>
-    <t>open_def2</t>
-  </si>
-  <si>
-    <t>Open Def 2</t>
-  </si>
-  <si>
-    <t>open_def2_badge</t>
-  </si>
-  <si>
-    <t>$open_def2</t>
-  </si>
-  <si>
-    <t>open_def3_btn</t>
-  </si>
-  <si>
-    <t>open_def3</t>
-  </si>
-  <si>
-    <t>Open Def 3</t>
-  </si>
-  <si>
-    <t>open_def3_badge</t>
-  </si>
-  <si>
-    <t>$open_def3</t>
-  </si>
-  <si>
-    <t>open_def4_btn</t>
-  </si>
-  <si>
-    <t>open_def4</t>
-  </si>
-  <si>
-    <t>Open Def 4</t>
-  </si>
-  <si>
-    <t>open_def4_badge</t>
-  </si>
-  <si>
-    <t>$open_def4</t>
-  </si>
-  <si>
-    <t>open_def5_btn</t>
-  </si>
-  <si>
-    <t>open_def5</t>
-  </si>
-  <si>
-    <t>Open Def 5</t>
-  </si>
-  <si>
-    <t>open_def5_badge</t>
-  </si>
-  <si>
-    <t>$open_def5</t>
-  </si>
-  <si>
-    <t>pick_ball_btn</t>
-  </si>
-  <si>
-    <t>pick_ball</t>
-  </si>
-  <si>
-    <t>Pick Ball</t>
-  </si>
-  <si>
     <t>pick_ball_badge</t>
   </si>
   <si>
-    <t>$pick_ball</t>
-  </si>
-  <si>
-    <t>pass_ball_btn</t>
-  </si>
-  <si>
-    <t>pass_ball</t>
-  </si>
-  <si>
-    <t>Pass Ball</t>
-  </si>
-  <si>
-    <t>pass_ball_badge</t>
-  </si>
-  <si>
-    <t>$pass_ball</t>
-  </si>
-  <si>
     <t>score_low</t>
   </si>
   <si>
@@ -1129,9 +919,6 @@
     <t>auto_fuel_high</t>
   </si>
   <si>
-    <t>telop_gears</t>
-  </si>
-  <si>
     <t>teleop_fuel_low</t>
   </si>
   <si>
@@ -1151,6 +938,201 @@
   </si>
   <si>
     <t>tech_fouls</t>
+  </si>
+  <si>
+    <t>auto_cross_line_btn</t>
+  </si>
+  <si>
+    <t>Cross Line</t>
+  </si>
+  <si>
+    <t>$auto_cross_line</t>
+  </si>
+  <si>
+    <t>$auto_gear_left</t>
+  </si>
+  <si>
+    <t>$auto_gear_center</t>
+  </si>
+  <si>
+    <t>$auto_gear_right</t>
+  </si>
+  <si>
+    <t>$auto_fuel_low</t>
+  </si>
+  <si>
+    <t>$auto_fuel_high</t>
+  </si>
+  <si>
+    <t>Gear Left</t>
+  </si>
+  <si>
+    <t>Gear Center</t>
+  </si>
+  <si>
+    <t>Gear Right</t>
+  </si>
+  <si>
+    <t>auto_gear_left_btn</t>
+  </si>
+  <si>
+    <t>auto_gear_center_btn</t>
+  </si>
+  <si>
+    <t>auto_gear_right_btn</t>
+  </si>
+  <si>
+    <t>auto_fuel_low_btn</t>
+  </si>
+  <si>
+    <t>auto_fuel_high_btn</t>
+  </si>
+  <si>
+    <t>Fuel High</t>
+  </si>
+  <si>
+    <t>Fuel Low</t>
+  </si>
+  <si>
+    <t>auto_fuel_low_badge</t>
+  </si>
+  <si>
+    <t>auto_fuel_high_badge</t>
+  </si>
+  <si>
+    <t>teleop_gears</t>
+  </si>
+  <si>
+    <t>gears_btn</t>
+  </si>
+  <si>
+    <t>gears</t>
+  </si>
+  <si>
+    <t>Gears</t>
+  </si>
+  <si>
+    <t>gears_badge</t>
+  </si>
+  <si>
+    <t>fuel_low_btn</t>
+  </si>
+  <si>
+    <t>fuel_high_btn</t>
+  </si>
+  <si>
+    <t>climb_btn</t>
+  </si>
+  <si>
+    <t>fuel_low</t>
+  </si>
+  <si>
+    <t>fuel_high</t>
+  </si>
+  <si>
+    <t>climb</t>
+  </si>
+  <si>
+    <t>fuel_low_badge</t>
+  </si>
+  <si>
+    <t>fuel_high_badge</t>
+  </si>
+  <si>
+    <t>$fuel_low</t>
+  </si>
+  <si>
+    <t>$fuel_high</t>
+  </si>
+  <si>
+    <t>$climb</t>
+  </si>
+  <si>
+    <t>Floor Gear</t>
+  </si>
+  <si>
+    <t>Floor Ball</t>
+  </si>
+  <si>
+    <t>floor_gear_btn</t>
+  </si>
+  <si>
+    <t>$floor_gear</t>
+  </si>
+  <si>
+    <t>floor_ball_btn</t>
+  </si>
+  <si>
+    <t>floor_ball</t>
+  </si>
+  <si>
+    <t>$floor_ball</t>
+  </si>
+  <si>
+    <t>Load From Hopper</t>
+  </si>
+  <si>
+    <t>pick_gear_badge</t>
+  </si>
+  <si>
+    <t>defense_badge</t>
+  </si>
+  <si>
+    <t>load_hopper_badge</t>
+  </si>
+  <si>
+    <t>$defense</t>
+  </si>
+  <si>
+    <t>$load_hopper</t>
+  </si>
+  <si>
+    <t>load_hopper</t>
+  </si>
+  <si>
+    <t>load_hopper_btn</t>
+  </si>
+  <si>
+    <t>defense_btn</t>
+  </si>
+  <si>
+    <t>fouls_btn</t>
+  </si>
+  <si>
+    <t>tech_fouls_btn</t>
+  </si>
+  <si>
+    <t>died_btn</t>
+  </si>
+  <si>
+    <t>Fouls</t>
+  </si>
+  <si>
+    <t>Tech Fouls</t>
+  </si>
+  <si>
+    <t>died_badge</t>
+  </si>
+  <si>
+    <t>tech_fouls_badge</t>
+  </si>
+  <si>
+    <t>fouls_badge</t>
+  </si>
+  <si>
+    <t>$fouls</t>
+  </si>
+  <si>
+    <t>$tech_fouls</t>
+  </si>
+  <si>
+    <t>$died</t>
+  </si>
+  <si>
+    <t>$gears</t>
+  </si>
+  <si>
+    <t>floor_gear</t>
   </si>
 </sst>
 </file>
@@ -1184,7 +1166,7 @@
       <name val="Source Code Pro"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1206,12 +1188,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFD8D8D8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1254,7 +1230,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -1268,7 +1244,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1601,20 +1576,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G31"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A18" sqref="A18:XFD18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26:XFD26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20" customWidth="1"/>
-    <col min="6" max="6" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="17.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1642,467 +1616,411 @@
       </c>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="11" t="s">
-        <v>11</v>
+      <c r="A2" s="5" t="s">
+        <v>307</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>293</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>308</v>
+      </c>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5" t="s">
+        <v>309</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>363</v>
+        <v>293</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>366</v>
+        <v>296</v>
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11" t="s">
-        <v>16</v>
+      <c r="A3" s="5" t="s">
+        <v>318</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>294</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>315</v>
+      </c>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5" t="s">
+        <v>310</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>364</v>
+        <v>294</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>366</v>
+        <v>296</v>
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11" t="s">
-        <v>20</v>
+      <c r="A4" s="5" t="s">
+        <v>319</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>295</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>316</v>
+      </c>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5" t="s">
+        <v>311</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>365</v>
+        <v>295</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>366</v>
+        <v>296</v>
       </c>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="B5" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="C5" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11" t="s">
-        <v>25</v>
+      <c r="A5" s="5" t="s">
+        <v>320</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>297</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>317</v>
+      </c>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5" t="s">
+        <v>312</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>367</v>
+        <v>297</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>366</v>
+        <v>296</v>
       </c>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="B6" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="C6" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11" t="s">
-        <v>30</v>
+      <c r="A6" s="5" t="s">
+        <v>321</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>298</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>324</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>325</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>313</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>368</v>
+        <v>298</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>366</v>
+        <v>296</v>
       </c>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="11"/>
-      <c r="B7" s="11"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
+      <c r="A7" s="5" t="s">
+        <v>322</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>299</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>323</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>326</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>314</v>
+      </c>
       <c r="F7" s="2" t="s">
-        <v>369</v>
+        <v>299</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>366</v>
+        <v>296</v>
       </c>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" s="11"/>
-      <c r="B8" s="11"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
+      <c r="A8" s="5"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="B9" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="C9" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="D9" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="E9" s="11" t="s">
-        <v>36</v>
+      <c r="A9" s="5" t="s">
+        <v>328</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>329</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>330</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>331</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>370</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>370</v>
+        <v>327</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:7">
-      <c r="A10" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="B10" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="C10" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="D10" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="E10" s="11" t="s">
-        <v>41</v>
+      <c r="A10" s="5" t="s">
+        <v>332</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>335</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>324</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>338</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>340</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>371</v>
+        <v>300</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:7">
-      <c r="A11" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="B11" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="C11" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="D11" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="E11" s="11" t="s">
-        <v>46</v>
+      <c r="A11" s="5" t="s">
+        <v>333</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>336</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>323</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>339</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>341</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>372</v>
+        <v>301</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:7">
-      <c r="A12" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="B12" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="C12" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="D12" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="E12" s="11" t="s">
-        <v>51</v>
+      <c r="A12" s="5" t="s">
+        <v>334</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>337</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>260</v>
+      </c>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5" t="s">
+        <v>342</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>373</v>
+        <v>302</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:7">
-      <c r="A13" s="11"/>
-      <c r="B13" s="11"/>
-      <c r="C13" s="11"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="11"/>
+      <c r="A13" s="5"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
     </row>
     <row r="14" spans="1:7">
-      <c r="A14" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="B14" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="C14" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="D14" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="E14" s="11" t="s">
-        <v>56</v>
+      <c r="A14" s="5" t="s">
+        <v>345</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>371</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>343</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>351</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>346</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>374</v>
+        <v>303</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="15" spans="1:7">
-      <c r="A15" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="B15" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="C15" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="D15" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="E15" s="11" t="s">
-        <v>61</v>
+      <c r="A15" s="5" t="s">
+        <v>347</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>348</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>344</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>349</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>375</v>
+        <v>304</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="16" spans="1:7">
-      <c r="A16" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="B16" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="C16" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="D16" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="E16" s="11" t="s">
-        <v>66</v>
+      <c r="A16" s="5" t="s">
+        <v>358</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>352</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>354</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>89</v>
+        <v>19</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="17" spans="1:7">
-      <c r="A17" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="B17" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="C17" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="D17" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="E17" s="11" t="s">
-        <v>71</v>
+      <c r="A17" s="5" t="s">
+        <v>357</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>356</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>350</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>353</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>355</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>376</v>
+        <v>305</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="18" spans="1:7">
-      <c r="A18" s="11"/>
-      <c r="B18" s="11"/>
-      <c r="C18" s="11"/>
-      <c r="D18" s="11"/>
-      <c r="E18" s="11"/>
+      <c r="A18" s="5"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
     </row>
     <row r="19" spans="1:7">
-      <c r="A19" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="B19" s="11" t="s">
-        <v>73</v>
-      </c>
-      <c r="C19" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="D19" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="E19" s="11" t="s">
-        <v>76</v>
+      <c r="A19" s="5" t="s">
+        <v>359</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>362</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>366</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>367</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>91</v>
+        <v>21</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="20" spans="1:7">
-      <c r="A20" s="11" t="s">
-        <v>77</v>
-      </c>
-      <c r="B20" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="C20" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="D20" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="E20" s="11" t="s">
-        <v>81</v>
+      <c r="A20" s="5" t="s">
+        <v>360</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>306</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>363</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>365</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>368</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>377</v>
+        <v>306</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="21" spans="1:7">
-      <c r="A21" s="11" t="s">
-        <v>82</v>
-      </c>
-      <c r="B21" s="11" t="s">
-        <v>83</v>
-      </c>
-      <c r="C21" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="D21" s="11" t="s">
-        <v>85</v>
-      </c>
-      <c r="E21" s="11" t="s">
-        <v>86</v>
+      <c r="A21" s="5" t="s">
+        <v>361</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>364</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>369</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>92</v>
+        <v>22</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7">
-      <c r="A24" t="s">
-        <v>94</v>
-      </c>
-      <c r="B24" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7">
-      <c r="A25" t="s">
-        <v>95</v>
-      </c>
-      <c r="B25" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7">
-      <c r="A26" t="s">
-        <v>96</v>
-      </c>
-      <c r="B26" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7">
-      <c r="A27" t="s">
-        <v>97</v>
-      </c>
-      <c r="B27" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7">
-      <c r="A28" t="s">
-        <v>98</v>
-      </c>
-      <c r="B28" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7">
-      <c r="A29" t="s">
-        <v>99</v>
-      </c>
-      <c r="B29" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7">
-      <c r="A30" t="s">
-        <v>100</v>
-      </c>
-      <c r="B30" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7">
-      <c r="A31" t="s">
-        <v>101</v>
-      </c>
-      <c r="B31" t="s">
-        <v>101</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -2131,210 +2049,210 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
-        <v>102</v>
+        <v>32</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>103</v>
+        <v>33</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>104</v>
+        <v>34</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>105</v>
+        <v>35</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>106</v>
+        <v>36</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>107</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="2" t="s">
-        <v>108</v>
+        <v>38</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>109</v>
+        <v>39</v>
       </c>
       <c r="C2" s="2">
         <f>LEN(B2)</f>
         <v>10</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>110</v>
+        <v>40</v>
       </c>
       <c r="E2" s="2">
         <f>LEN(D2)</f>
         <v>12</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>111</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="2" t="s">
-        <v>108</v>
+        <v>38</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>112</v>
+        <v>42</v>
       </c>
       <c r="C3" s="2">
         <f t="shared" ref="C3:E9" si="0">LEN(B3)</f>
         <v>6</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>113</v>
+        <v>43</v>
       </c>
       <c r="E3" s="2">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>114</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="2" t="s">
-        <v>115</v>
+        <v>45</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>116</v>
+        <v>46</v>
       </c>
       <c r="C4" s="2">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>117</v>
+        <v>47</v>
       </c>
       <c r="E4" s="2">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>118</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="2" t="s">
-        <v>115</v>
+        <v>45</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>119</v>
+        <v>49</v>
       </c>
       <c r="C5" s="2">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>120</v>
+        <v>50</v>
       </c>
       <c r="E5" s="2">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>121</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="2" t="s">
-        <v>122</v>
+        <v>52</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>123</v>
+        <v>53</v>
       </c>
       <c r="C6" s="2">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>124</v>
+        <v>54</v>
       </c>
       <c r="E6" s="2">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>125</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="2" t="s">
-        <v>122</v>
+        <v>52</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>126</v>
+        <v>56</v>
       </c>
       <c r="C7" s="2">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>127</v>
+        <v>57</v>
       </c>
       <c r="E7" s="2">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>128</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="2" t="s">
-        <v>129</v>
+        <v>59</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>130</v>
+        <v>60</v>
       </c>
       <c r="C8" s="2">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>131</v>
+        <v>61</v>
       </c>
       <c r="E8" s="2">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>132</v>
+        <v>62</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="2" t="s">
-        <v>129</v>
+        <v>59</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>133</v>
+        <v>63</v>
       </c>
       <c r="C9" s="2">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>134</v>
+        <v>64</v>
       </c>
       <c r="E9" s="2">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>135</v>
+        <v>65</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="B10" t="s">
-        <v>136</v>
+        <v>66</v>
       </c>
       <c r="C10" s="9">
         <f>MAX(C2:C9)</f>
         <v>13</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>136</v>
+        <v>66</v>
       </c>
       <c r="E10" s="9">
         <f>MAX(E2:E9)</f>
@@ -2367,788 +2285,788 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" s="4" t="s">
-        <v>137</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" s="4" t="s">
-        <v>138</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" s="4" t="s">
-        <v>139</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="4" t="s">
-        <v>140</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="4" t="s">
-        <v>141</v>
+        <v>71</v>
       </c>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="4" t="s">
-        <v>142</v>
+        <v>72</v>
       </c>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="4" t="s">
-        <v>143</v>
+        <v>73</v>
       </c>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="4" t="s">
-        <v>144</v>
+        <v>74</v>
       </c>
     </row>
     <row r="9" spans="1:10">
       <c r="A9" s="4" t="s">
-        <v>145</v>
+        <v>75</v>
       </c>
     </row>
     <row r="10" spans="1:10">
       <c r="A10" s="4" t="s">
-        <v>146</v>
+        <v>76</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>147</v>
+        <v>77</v>
       </c>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="4" t="s">
-        <v>148</v>
+        <v>78</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>149</v>
+        <v>79</v>
       </c>
     </row>
     <row r="12" spans="1:10">
       <c r="A12" s="4" t="s">
-        <v>150</v>
+        <v>80</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>151</v>
+        <v>81</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>31</v>
+        <v>10</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>152</v>
+        <v>82</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>153</v>
+        <v>83</v>
       </c>
     </row>
     <row r="13" spans="1:10">
       <c r="A13" s="4" t="s">
-        <v>154</v>
+        <v>84</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>155</v>
+        <v>85</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>156</v>
+        <v>86</v>
       </c>
       <c r="J13" s="3" t="s">
-        <v>157</v>
+        <v>87</v>
       </c>
     </row>
     <row r="14" spans="1:10">
       <c r="A14" s="4" t="s">
-        <v>158</v>
+        <v>88</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>159</v>
+        <v>89</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>160</v>
+        <v>90</v>
       </c>
       <c r="J14" s="3" t="s">
-        <v>161</v>
+        <v>91</v>
       </c>
     </row>
     <row r="15" spans="1:10">
       <c r="A15" s="4" t="s">
-        <v>162</v>
+        <v>92</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>163</v>
+        <v>93</v>
       </c>
     </row>
     <row r="16" spans="1:10">
       <c r="A16" s="4" t="s">
-        <v>164</v>
+        <v>94</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>165</v>
+        <v>95</v>
       </c>
     </row>
     <row r="17" spans="1:10">
       <c r="A17" s="4" t="s">
-        <v>166</v>
+        <v>96</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>167</v>
+        <v>97</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>168</v>
+        <v>98</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>169</v>
+        <v>99</v>
       </c>
       <c r="J17" s="3" t="s">
-        <v>170</v>
+        <v>100</v>
       </c>
     </row>
     <row r="18" spans="1:10">
       <c r="A18" s="4" t="s">
-        <v>171</v>
+        <v>101</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>172</v>
+        <v>102</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>173</v>
+        <v>103</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>174</v>
+        <v>104</v>
       </c>
       <c r="J18" s="3" t="s">
-        <v>175</v>
+        <v>105</v>
       </c>
     </row>
     <row r="19" spans="1:10">
       <c r="A19" s="4" t="s">
-        <v>176</v>
+        <v>106</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>177</v>
+        <v>107</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>91</v>
+        <v>21</v>
       </c>
       <c r="I19" s="3" t="s">
-        <v>178</v>
+        <v>108</v>
       </c>
       <c r="J19" s="3" t="s">
-        <v>179</v>
+        <v>109</v>
       </c>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="4" t="s">
-        <v>180</v>
+        <v>110</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>181</v>
+        <v>111</v>
       </c>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="4" t="s">
-        <v>182</v>
+        <v>112</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>183</v>
+        <v>113</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>33</v>
+        <v>11</v>
       </c>
       <c r="I21" s="3" t="s">
-        <v>184</v>
+        <v>114</v>
       </c>
       <c r="J21" s="3" t="s">
-        <v>185</v>
+        <v>115</v>
       </c>
     </row>
     <row r="22" spans="1:10">
       <c r="A22" s="4" t="s">
-        <v>186</v>
+        <v>116</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>187</v>
+        <v>117</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>188</v>
+        <v>118</v>
       </c>
       <c r="I22" s="3" t="s">
-        <v>94</v>
+        <v>24</v>
       </c>
       <c r="J22" s="3" t="s">
-        <v>98</v>
+        <v>28</v>
       </c>
     </row>
     <row r="23" spans="1:10">
       <c r="A23" s="4" t="s">
-        <v>189</v>
+        <v>119</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>190</v>
+        <v>120</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>38</v>
+        <v>12</v>
       </c>
       <c r="I23" s="3" t="s">
-        <v>191</v>
+        <v>121</v>
       </c>
       <c r="J23" s="3" t="s">
-        <v>192</v>
+        <v>122</v>
       </c>
     </row>
     <row r="24" spans="1:10">
       <c r="A24" s="4" t="s">
-        <v>193</v>
+        <v>123</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>194</v>
+        <v>124</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>195</v>
+        <v>125</v>
       </c>
       <c r="I24" s="3" t="s">
-        <v>95</v>
+        <v>25</v>
       </c>
       <c r="J24" s="3" t="s">
-        <v>99</v>
+        <v>29</v>
       </c>
     </row>
     <row r="25" spans="1:10">
       <c r="A25" s="4" t="s">
-        <v>196</v>
+        <v>126</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>197</v>
+        <v>127</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>43</v>
+        <v>13</v>
       </c>
       <c r="I25" s="3" t="s">
-        <v>198</v>
+        <v>128</v>
       </c>
       <c r="J25" s="3" t="s">
-        <v>199</v>
+        <v>129</v>
       </c>
     </row>
     <row r="26" spans="1:10">
       <c r="A26" s="4" t="s">
-        <v>200</v>
+        <v>130</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>201</v>
+        <v>131</v>
       </c>
       <c r="H26" s="3" t="s">
-        <v>202</v>
+        <v>132</v>
       </c>
       <c r="I26" s="3" t="s">
-        <v>96</v>
+        <v>26</v>
       </c>
       <c r="J26" s="3" t="s">
-        <v>100</v>
+        <v>30</v>
       </c>
     </row>
     <row r="27" spans="1:10">
       <c r="A27" s="4" t="s">
-        <v>203</v>
+        <v>133</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>204</v>
+        <v>134</v>
       </c>
       <c r="H27" s="3" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="I27" s="3" t="s">
-        <v>205</v>
+        <v>135</v>
       </c>
       <c r="J27" s="3" t="s">
-        <v>206</v>
+        <v>136</v>
       </c>
     </row>
     <row r="28" spans="1:10">
       <c r="A28" s="4" t="s">
-        <v>207</v>
+        <v>137</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>208</v>
+        <v>138</v>
       </c>
       <c r="H28" s="3" t="s">
-        <v>209</v>
+        <v>139</v>
       </c>
       <c r="I28" s="3" t="s">
-        <v>97</v>
+        <v>27</v>
       </c>
       <c r="J28" s="3" t="s">
-        <v>101</v>
+        <v>31</v>
       </c>
     </row>
     <row r="29" spans="1:10">
       <c r="A29" s="4" t="s">
-        <v>210</v>
+        <v>140</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>211</v>
+        <v>141</v>
       </c>
       <c r="H29" s="3" t="s">
-        <v>53</v>
+        <v>15</v>
       </c>
       <c r="I29" s="3" t="s">
-        <v>212</v>
+        <v>142</v>
       </c>
       <c r="J29" s="3" t="s">
-        <v>213</v>
+        <v>143</v>
       </c>
     </row>
     <row r="30" spans="1:10">
       <c r="A30" s="4" t="s">
-        <v>214</v>
+        <v>144</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>215</v>
+        <v>145</v>
       </c>
       <c r="H30" s="3" t="s">
-        <v>216</v>
+        <v>146</v>
       </c>
       <c r="I30" s="3" t="s">
-        <v>217</v>
+        <v>147</v>
       </c>
       <c r="J30" s="3" t="s">
-        <v>218</v>
+        <v>148</v>
       </c>
     </row>
     <row r="31" spans="1:10">
       <c r="A31" s="4" t="s">
-        <v>219</v>
+        <v>149</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>220</v>
+        <v>150</v>
       </c>
       <c r="H31" s="3" t="s">
-        <v>221</v>
+        <v>151</v>
       </c>
       <c r="I31" s="3" t="s">
-        <v>222</v>
+        <v>152</v>
       </c>
       <c r="J31" s="3" t="s">
-        <v>223</v>
+        <v>153</v>
       </c>
     </row>
     <row r="32" spans="1:10">
       <c r="A32" s="4" t="s">
-        <v>224</v>
+        <v>154</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>225</v>
+        <v>155</v>
       </c>
       <c r="H32" s="3" t="s">
-        <v>226</v>
+        <v>156</v>
       </c>
       <c r="I32" s="3" t="s">
-        <v>227</v>
+        <v>157</v>
       </c>
       <c r="J32" s="3" t="s">
-        <v>228</v>
+        <v>158</v>
       </c>
     </row>
     <row r="33" spans="1:10">
       <c r="A33" s="4" t="s">
-        <v>229</v>
+        <v>159</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>230</v>
+        <v>160</v>
       </c>
     </row>
     <row r="34" spans="1:10">
       <c r="A34" s="4" t="s">
-        <v>231</v>
+        <v>161</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>232</v>
+        <v>162</v>
       </c>
     </row>
     <row r="35" spans="1:10">
       <c r="A35" s="4" t="s">
-        <v>233</v>
+        <v>163</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>234</v>
+        <v>164</v>
       </c>
       <c r="H35" s="3" t="s">
-        <v>88</v>
+        <v>18</v>
       </c>
       <c r="I35" s="3" t="s">
-        <v>235</v>
+        <v>165</v>
       </c>
       <c r="J35" s="3" t="s">
-        <v>236</v>
+        <v>166</v>
       </c>
     </row>
     <row r="36" spans="1:10">
       <c r="A36" s="4" t="s">
-        <v>237</v>
+        <v>167</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>238</v>
+        <v>168</v>
       </c>
       <c r="H36" s="3" t="s">
-        <v>87</v>
+        <v>17</v>
       </c>
       <c r="I36" s="3" t="s">
-        <v>239</v>
+        <v>169</v>
       </c>
       <c r="J36" s="3" t="s">
-        <v>240</v>
+        <v>170</v>
       </c>
     </row>
     <row r="37" spans="1:10">
       <c r="A37" s="4" t="s">
-        <v>241</v>
+        <v>171</v>
       </c>
       <c r="G37" s="3" t="s">
-        <v>242</v>
+        <v>172</v>
       </c>
     </row>
     <row r="38" spans="1:10">
       <c r="A38" s="4" t="s">
-        <v>243</v>
+        <v>173</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>244</v>
+        <v>174</v>
       </c>
     </row>
     <row r="39" spans="1:10">
       <c r="A39" s="4" t="s">
-        <v>245</v>
+        <v>175</v>
       </c>
       <c r="G39" s="3" t="s">
-        <v>246</v>
+        <v>176</v>
       </c>
     </row>
     <row r="40" spans="1:10">
       <c r="A40" s="4" t="s">
-        <v>247</v>
+        <v>177</v>
       </c>
       <c r="G40" s="3" t="s">
-        <v>248</v>
+        <v>178</v>
       </c>
     </row>
     <row r="41" spans="1:10">
       <c r="A41" s="4" t="s">
-        <v>249</v>
+        <v>179</v>
       </c>
       <c r="G41" s="3" t="s">
-        <v>250</v>
+        <v>180</v>
       </c>
     </row>
     <row r="42" spans="1:10">
       <c r="A42" s="4" t="s">
-        <v>251</v>
+        <v>181</v>
       </c>
       <c r="G42" s="3" t="s">
-        <v>252</v>
+        <v>182</v>
       </c>
     </row>
     <row r="43" spans="1:10">
       <c r="A43" s="4" t="s">
-        <v>253</v>
+        <v>183</v>
       </c>
       <c r="G43" s="3" t="s">
-        <v>254</v>
+        <v>184</v>
       </c>
     </row>
     <row r="44" spans="1:10">
       <c r="A44" s="4" t="s">
-        <v>255</v>
+        <v>185</v>
       </c>
       <c r="G44" s="3" t="s">
-        <v>256</v>
+        <v>186</v>
       </c>
     </row>
     <row r="45" spans="1:10">
       <c r="A45" s="4" t="s">
-        <v>257</v>
+        <v>187</v>
       </c>
       <c r="G45" s="3" t="s">
-        <v>258</v>
+        <v>188</v>
       </c>
       <c r="H45" s="3" t="s">
-        <v>259</v>
+        <v>189</v>
       </c>
       <c r="I45" s="3" t="s">
-        <v>260</v>
+        <v>190</v>
       </c>
       <c r="J45" s="3" t="s">
-        <v>261</v>
+        <v>191</v>
       </c>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="4" t="s">
-        <v>262</v>
+        <v>192</v>
       </c>
       <c r="G46" s="3" t="s">
-        <v>263</v>
+        <v>193</v>
       </c>
       <c r="H46" s="3" t="s">
-        <v>264</v>
+        <v>194</v>
       </c>
       <c r="I46" s="3" t="s">
-        <v>265</v>
+        <v>195</v>
       </c>
       <c r="J46" s="3" t="s">
-        <v>266</v>
+        <v>196</v>
       </c>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="4" t="s">
-        <v>267</v>
+        <v>197</v>
       </c>
       <c r="G47" s="3" t="s">
-        <v>268</v>
+        <v>198</v>
       </c>
       <c r="H47" s="3" t="s">
-        <v>269</v>
+        <v>199</v>
       </c>
       <c r="I47" s="3" t="s">
-        <v>270</v>
+        <v>200</v>
       </c>
       <c r="J47" s="3" t="s">
-        <v>271</v>
+        <v>201</v>
       </c>
     </row>
     <row r="48" spans="1:10">
       <c r="A48" s="4" t="s">
-        <v>272</v>
+        <v>202</v>
       </c>
     </row>
     <row r="49" spans="1:1">
       <c r="A49" s="4" t="s">
-        <v>144</v>
+        <v>74</v>
       </c>
     </row>
     <row r="50" spans="1:1">
       <c r="A50" s="4" t="s">
-        <v>145</v>
+        <v>75</v>
       </c>
     </row>
     <row r="51" spans="1:1">
       <c r="A51" s="4" t="s">
-        <v>273</v>
+        <v>203</v>
       </c>
     </row>
     <row r="52" spans="1:1">
       <c r="A52" s="4" t="s">
-        <v>148</v>
+        <v>78</v>
       </c>
     </row>
     <row r="53" spans="1:1">
       <c r="A53" s="4" t="s">
-        <v>150</v>
+        <v>80</v>
       </c>
     </row>
     <row r="54" spans="1:1">
       <c r="A54" s="4" t="s">
-        <v>154</v>
+        <v>84</v>
       </c>
     </row>
     <row r="55" spans="1:1">
       <c r="A55" s="4" t="s">
-        <v>158</v>
+        <v>88</v>
       </c>
     </row>
     <row r="56" spans="1:1">
       <c r="A56" s="4" t="s">
-        <v>162</v>
+        <v>92</v>
       </c>
     </row>
     <row r="57" spans="1:1">
       <c r="A57" s="4" t="s">
-        <v>164</v>
+        <v>94</v>
       </c>
     </row>
     <row r="58" spans="1:1">
       <c r="A58" s="4" t="s">
-        <v>166</v>
+        <v>96</v>
       </c>
     </row>
     <row r="59" spans="1:1">
       <c r="A59" s="4" t="s">
-        <v>171</v>
+        <v>101</v>
       </c>
     </row>
     <row r="60" spans="1:1">
       <c r="A60" s="4" t="s">
-        <v>176</v>
+        <v>106</v>
       </c>
     </row>
     <row r="61" spans="1:1">
       <c r="A61" s="4" t="s">
-        <v>180</v>
+        <v>110</v>
       </c>
     </row>
     <row r="62" spans="1:1">
       <c r="A62" s="4" t="s">
-        <v>182</v>
+        <v>112</v>
       </c>
     </row>
     <row r="63" spans="1:1">
       <c r="A63" s="4" t="s">
-        <v>274</v>
+        <v>204</v>
       </c>
     </row>
     <row r="64" spans="1:1">
       <c r="A64" s="4" t="s">
-        <v>275</v>
+        <v>205</v>
       </c>
     </row>
     <row r="65" spans="1:1">
       <c r="A65" s="4" t="s">
-        <v>276</v>
+        <v>206</v>
       </c>
     </row>
     <row r="66" spans="1:1">
       <c r="A66" s="4" t="s">
-        <v>277</v>
+        <v>207</v>
       </c>
     </row>
     <row r="67" spans="1:1">
       <c r="A67" s="4" t="s">
-        <v>278</v>
+        <v>208</v>
       </c>
     </row>
     <row r="68" spans="1:1">
       <c r="A68" s="4" t="s">
-        <v>279</v>
+        <v>209</v>
       </c>
     </row>
     <row r="69" spans="1:1">
       <c r="A69" s="4" t="s">
-        <v>280</v>
+        <v>210</v>
       </c>
     </row>
     <row r="70" spans="1:1">
       <c r="A70" s="4" t="s">
-        <v>281</v>
+        <v>211</v>
       </c>
     </row>
     <row r="71" spans="1:1">
       <c r="A71" s="4" t="s">
-        <v>214</v>
+        <v>144</v>
       </c>
     </row>
     <row r="72" spans="1:1">
       <c r="A72" s="4" t="s">
-        <v>282</v>
+        <v>212</v>
       </c>
     </row>
     <row r="73" spans="1:1">
       <c r="A73" s="4" t="s">
-        <v>283</v>
+        <v>213</v>
       </c>
     </row>
     <row r="74" spans="1:1">
       <c r="A74" s="4" t="s">
-        <v>229</v>
+        <v>159</v>
       </c>
     </row>
     <row r="75" spans="1:1">
       <c r="A75" s="4" t="s">
-        <v>231</v>
+        <v>161</v>
       </c>
     </row>
     <row r="76" spans="1:1">
       <c r="A76" s="4" t="s">
-        <v>233</v>
+        <v>163</v>
       </c>
     </row>
     <row r="77" spans="1:1">
       <c r="A77" s="4" t="s">
-        <v>237</v>
+        <v>167</v>
       </c>
     </row>
     <row r="78" spans="1:1">
       <c r="A78" s="4" t="s">
-        <v>241</v>
+        <v>171</v>
       </c>
     </row>
     <row r="79" spans="1:1">
       <c r="A79" s="4" t="s">
-        <v>243</v>
+        <v>173</v>
       </c>
     </row>
     <row r="80" spans="1:1">
       <c r="A80" s="4" t="s">
-        <v>284</v>
+        <v>214</v>
       </c>
     </row>
     <row r="81" spans="1:1">
       <c r="A81" s="4" t="s">
-        <v>247</v>
+        <v>177</v>
       </c>
     </row>
     <row r="82" spans="1:1">
       <c r="A82" s="4" t="s">
-        <v>249</v>
+        <v>179</v>
       </c>
     </row>
     <row r="83" spans="1:1">
       <c r="A83" s="4" t="s">
-        <v>251</v>
+        <v>181</v>
       </c>
     </row>
     <row r="84" spans="1:1">
       <c r="A84" s="4" t="s">
-        <v>253</v>
+        <v>183</v>
       </c>
     </row>
     <row r="85" spans="1:1">
       <c r="A85" s="4" t="s">
-        <v>255</v>
+        <v>185</v>
       </c>
     </row>
     <row r="86" spans="1:1">
       <c r="A86" s="4" t="s">
-        <v>285</v>
+        <v>215</v>
       </c>
     </row>
     <row r="87" spans="1:1">
       <c r="A87" s="4" t="s">
-        <v>286</v>
+        <v>216</v>
       </c>
     </row>
     <row r="88" spans="1:1">
       <c r="A88" s="4" t="s">
-        <v>287</v>
+        <v>217</v>
       </c>
     </row>
     <row r="89" spans="1:1">
       <c r="A89" s="4" t="s">
-        <v>272</v>
+        <v>202</v>
       </c>
     </row>
     <row r="90" spans="1:1">
       <c r="A90" s="4" t="s">
-        <v>288</v>
+        <v>218</v>
       </c>
     </row>
     <row r="91" spans="1:1">
       <c r="A91" s="4" t="s">
-        <v>289</v>
+        <v>219</v>
       </c>
     </row>
     <row r="92" spans="1:1">
       <c r="A92" s="4" t="s">
-        <v>290</v>
+        <v>220</v>
       </c>
     </row>
     <row r="93" spans="1:1">
       <c r="A93" s="4" t="s">
-        <v>291</v>
+        <v>221</v>
       </c>
     </row>
   </sheetData>
@@ -3161,7 +3079,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
@@ -3175,354 +3093,354 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
+        <v>222</v>
+      </c>
+      <c r="B1" t="s">
+        <v>223</v>
+      </c>
+      <c r="C1" t="s">
         <v>292</v>
-      </c>
-      <c r="B1" t="s">
-        <v>293</v>
-      </c>
-      <c r="C1" t="s">
-        <v>362</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>294</v>
+        <v>224</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="10" t="s">
-        <v>295</v>
+        <v>225</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>296</v>
+        <v>226</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="2" t="s">
-        <v>297</v>
+        <v>227</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>298</v>
+        <v>228</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="2" t="s">
-        <v>215</v>
+        <v>145</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>299</v>
+        <v>229</v>
       </c>
       <c r="C6" t="s">
-        <v>300</v>
+        <v>230</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="2" t="s">
-        <v>220</v>
+        <v>150</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>301</v>
+        <v>231</v>
       </c>
       <c r="C7" t="s">
-        <v>302</v>
+        <v>232</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="2" t="s">
-        <v>225</v>
+        <v>155</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>303</v>
+        <v>233</v>
       </c>
       <c r="C8" t="s">
-        <v>304</v>
+        <v>234</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" t="s">
-        <v>305</v>
+        <v>235</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="2" t="s">
-        <v>306</v>
+        <v>236</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>307</v>
+        <v>237</v>
       </c>
       <c r="C10" t="s">
-        <v>308</v>
+        <v>238</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="2" t="s">
-        <v>309</v>
+        <v>239</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>307</v>
+        <v>237</v>
       </c>
       <c r="C11" t="s">
-        <v>310</v>
+        <v>240</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="2" t="s">
-        <v>311</v>
+        <v>241</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>312</v>
+        <v>242</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="2" t="s">
-        <v>313</v>
+        <v>243</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>312</v>
+        <v>242</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="2" t="s">
-        <v>314</v>
+        <v>244</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>315</v>
+        <v>245</v>
       </c>
       <c r="C14" t="s">
-        <v>316</v>
+        <v>246</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="2" t="s">
-        <v>317</v>
+        <v>247</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>315</v>
+        <v>245</v>
       </c>
       <c r="C15" t="s">
-        <v>318</v>
+        <v>248</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="2" t="s">
-        <v>319</v>
+        <v>249</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>315</v>
+        <v>245</v>
       </c>
       <c r="C16" t="s">
-        <v>320</v>
+        <v>250</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="2" t="s">
-        <v>321</v>
+        <v>251</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>315</v>
+        <v>245</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="2" t="s">
-        <v>322</v>
+        <v>252</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>307</v>
+        <v>237</v>
       </c>
       <c r="C18" t="s">
-        <v>323</v>
+        <v>253</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="2" t="s">
-        <v>324</v>
+        <v>254</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>307</v>
+        <v>237</v>
       </c>
       <c r="C19" t="s">
-        <v>325</v>
+        <v>255</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" s="2" t="s">
-        <v>326</v>
+        <v>256</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>327</v>
+        <v>257</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" s="2" t="s">
-        <v>328</v>
+        <v>258</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>329</v>
+        <v>259</v>
       </c>
       <c r="C21" t="s">
-        <v>330</v>
+        <v>260</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" s="2" t="s">
-        <v>331</v>
+        <v>261</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>332</v>
+        <v>262</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" s="2" t="s">
-        <v>333</v>
+        <v>263</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>334</v>
+        <v>264</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" s="2" t="s">
-        <v>335</v>
+        <v>265</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>334</v>
+        <v>264</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" s="2" t="s">
-        <v>177</v>
+        <v>107</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>336</v>
+        <v>266</v>
       </c>
       <c r="C25" t="s">
-        <v>337</v>
+        <v>267</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" s="2" t="s">
-        <v>230</v>
+        <v>160</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>338</v>
+        <v>268</v>
       </c>
       <c r="C26" t="s">
-        <v>339</v>
+        <v>269</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" s="2" t="s">
-        <v>163</v>
+        <v>93</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>340</v>
+        <v>270</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" s="2" t="s">
-        <v>341</v>
+        <v>271</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>342</v>
+        <v>272</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" s="2" t="s">
-        <v>343</v>
+        <v>273</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>344</v>
+        <v>274</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" s="2" t="s">
-        <v>345</v>
+        <v>275</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>346</v>
+        <v>276</v>
       </c>
     </row>
     <row r="31" spans="1:3">
       <c r="A31" s="2" t="s">
-        <v>248</v>
+        <v>178</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>347</v>
+        <v>277</v>
       </c>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" s="2" t="s">
-        <v>348</v>
+        <v>278</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>349</v>
+        <v>279</v>
       </c>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" s="2" t="s">
-        <v>350</v>
+        <v>280</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>351</v>
+        <v>281</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" s="2" t="s">
-        <v>352</v>
+        <v>282</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>353</v>
+        <v>283</v>
       </c>
     </row>
     <row r="35" spans="1:3">
       <c r="A35" s="2" t="s">
-        <v>354</v>
+        <v>284</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>355</v>
+        <v>285</v>
       </c>
     </row>
     <row r="36" spans="1:3">
       <c r="A36" s="2" t="s">
-        <v>356</v>
+        <v>286</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>357</v>
+        <v>287</v>
       </c>
     </row>
     <row r="37" spans="1:3">
       <c r="A37" s="2" t="s">
-        <v>358</v>
+        <v>288</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>359</v>
+        <v>289</v>
       </c>
     </row>
     <row r="38" spans="1:3">
       <c r="A38" s="2" t="s">
-        <v>181</v>
+        <v>111</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>360</v>
+        <v>290</v>
       </c>
     </row>
     <row r="39" spans="1:3">
       <c r="A39" s="2" t="s">
-        <v>254</v>
+        <v>184</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>361</v>
+        <v>291</v>
       </c>
     </row>
     <row r="40" spans="1:3">
       <c r="C40" t="s">
-        <v>90</v>
+        <v>20</v>
       </c>
     </row>
     <row r="41" spans="1:3">
       <c r="C41" t="s">
-        <v>93</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Can now save stat
</commit_message>
<xml_diff>
--- a/docs/Reference.xlsx
+++ b/docs/Reference.xlsx
@@ -8,16 +8,15 @@
   </bookViews>
   <sheets>
     <sheet name="Reference" sheetId="1" r:id="rId1"/>
-    <sheet name="Defenses" sheetId="2" r:id="rId2"/>
-    <sheet name="matchScore2016" sheetId="4" r:id="rId3"/>
-    <sheet name="Score_2017" sheetId="5" r:id="rId4"/>
+    <sheet name="matchScore2016" sheetId="4" r:id="rId2"/>
+    <sheet name="Score_2017" sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="451" uniqueCount="372">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="337">
   <si>
     <t>Button Id</t>
   </si>
@@ -113,111 +112,6 @@
   </si>
   <si>
     <t>blue_def5</t>
-  </si>
-  <si>
-    <t>Category</t>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Name Length</t>
-  </si>
-  <si>
-    <t>API Name</t>
-  </si>
-  <si>
-    <t>API Name Length</t>
-  </si>
-  <si>
-    <t>avg_cross_low_bar</t>
-  </si>
-  <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>Portcullis</t>
-  </si>
-  <si>
-    <t>A_Portcullis</t>
-  </si>
-  <si>
-    <t>avg_cross_portcullis</t>
-  </si>
-  <si>
-    <t>Cheval</t>
-  </si>
-  <si>
-    <t>A_ChevalDeFrise</t>
-  </si>
-  <si>
-    <t>avg_cross_cheval</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
-    <t>Moat</t>
-  </si>
-  <si>
-    <t>B_Ramparts</t>
-  </si>
-  <si>
-    <t>avg_cross_ramparts</t>
-  </si>
-  <si>
-    <t>Ramparts</t>
-  </si>
-  <si>
-    <t>B_Moat</t>
-  </si>
-  <si>
-    <t>avg_cross_moat</t>
-  </si>
-  <si>
-    <t>C</t>
-  </si>
-  <si>
-    <t>Drawbridge</t>
-  </si>
-  <si>
-    <t>C_SallyPort</t>
-  </si>
-  <si>
-    <t>avg_cross_sallyport</t>
-  </si>
-  <si>
-    <t>Sally Port</t>
-  </si>
-  <si>
-    <t>C_Drawbridge</t>
-  </si>
-  <si>
-    <t>avg_cross_drawbridge</t>
-  </si>
-  <si>
-    <t>D</t>
-  </si>
-  <si>
-    <t>Rock Wall</t>
-  </si>
-  <si>
-    <t>D_RockWall</t>
-  </si>
-  <si>
-    <t>avg_cross_rockwall</t>
-  </si>
-  <si>
-    <t>Rough Terrain</t>
-  </si>
-  <si>
-    <t>D_RoughTerrain</t>
-  </si>
-  <si>
-    <t>avg_cross_rough</t>
-  </si>
-  <si>
-    <t>Max Length</t>
   </si>
   <si>
     <t>&lt;z:anyType xmlns:z="http://schemas.microsoft.com/2003/10/Serialization/" xmlns:i="http://www.w3.org/2001/XMLSchema-instance" i:type="EventScoreDetails"&gt;</t>
@@ -1166,7 +1060,7 @@
       <name val="Source Code Pro"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1181,18 +1075,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFD8D8D8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -1215,22 +1103,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -1239,11 +1116,7 @@
       <alignment horizontal="left" vertical="center" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1617,132 +1490,132 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="5" t="s">
-        <v>307</v>
+        <v>272</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>293</v>
+        <v>258</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>308</v>
+        <v>273</v>
       </c>
       <c r="D2" s="5"/>
       <c r="E2" s="5" t="s">
-        <v>309</v>
+        <v>274</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>293</v>
+        <v>258</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>296</v>
+        <v>261</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="5" t="s">
-        <v>318</v>
+        <v>283</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>294</v>
+        <v>259</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>315</v>
+        <v>280</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="5" t="s">
-        <v>310</v>
+        <v>275</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>294</v>
+        <v>259</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>296</v>
+        <v>261</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="5" t="s">
-        <v>319</v>
+        <v>284</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>295</v>
+        <v>260</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>316</v>
+        <v>281</v>
       </c>
       <c r="D4" s="5"/>
       <c r="E4" s="5" t="s">
-        <v>311</v>
+        <v>276</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>295</v>
+        <v>260</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>296</v>
+        <v>261</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="5" t="s">
-        <v>320</v>
+        <v>285</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>297</v>
+        <v>262</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>317</v>
+        <v>282</v>
       </c>
       <c r="D5" s="5"/>
       <c r="E5" s="5" t="s">
-        <v>312</v>
+        <v>277</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>297</v>
+        <v>262</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>296</v>
+        <v>261</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="5" t="s">
-        <v>321</v>
+        <v>286</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>298</v>
+        <v>263</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>324</v>
+        <v>289</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>325</v>
+        <v>290</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>313</v>
+        <v>278</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>298</v>
+        <v>263</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>296</v>
+        <v>261</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="5" t="s">
-        <v>322</v>
+        <v>287</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>299</v>
+        <v>264</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>323</v>
+        <v>288</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>326</v>
+        <v>291</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>314</v>
+        <v>279</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>299</v>
+        <v>264</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>296</v>
+        <v>261</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -1756,22 +1629,22 @@
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="5" t="s">
-        <v>328</v>
+        <v>293</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>329</v>
+        <v>294</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>330</v>
+        <v>295</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>331</v>
+        <v>296</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>370</v>
+        <v>335</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>327</v>
+        <v>292</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>7</v>
@@ -1779,22 +1652,22 @@
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="5" t="s">
-        <v>332</v>
+        <v>297</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>335</v>
+        <v>300</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>324</v>
+        <v>289</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>338</v>
+        <v>303</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>340</v>
+        <v>305</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>300</v>
+        <v>265</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>7</v>
@@ -1802,22 +1675,22 @@
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="5" t="s">
-        <v>333</v>
+        <v>298</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>336</v>
+        <v>301</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>323</v>
+        <v>288</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>339</v>
+        <v>304</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>341</v>
+        <v>306</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>301</v>
+        <v>266</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>7</v>
@@ -1825,20 +1698,20 @@
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="5" t="s">
-        <v>334</v>
+        <v>299</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>337</v>
+        <v>302</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>260</v>
+        <v>225</v>
       </c>
       <c r="D12" s="5"/>
       <c r="E12" s="5" t="s">
-        <v>342</v>
+        <v>307</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>302</v>
+        <v>267</v>
       </c>
       <c r="G12" s="2" t="s">
         <v>7</v>
@@ -1855,22 +1728,22 @@
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="5" t="s">
-        <v>345</v>
+        <v>310</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>371</v>
+        <v>336</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>343</v>
+        <v>308</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>351</v>
+        <v>316</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>346</v>
+        <v>311</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>303</v>
+        <v>268</v>
       </c>
       <c r="G14" s="2" t="s">
         <v>7</v>
@@ -1878,22 +1751,22 @@
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="5" t="s">
-        <v>347</v>
+        <v>312</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>348</v>
+        <v>313</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>344</v>
+        <v>309</v>
       </c>
       <c r="D15" s="5" t="s">
         <v>16</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>349</v>
+        <v>314</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>304</v>
+        <v>269</v>
       </c>
       <c r="G15" s="2" t="s">
         <v>7</v>
@@ -1901,7 +1774,7 @@
     </row>
     <row r="16" spans="1:7">
       <c r="A16" s="5" t="s">
-        <v>358</v>
+        <v>323</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>19</v>
@@ -1910,10 +1783,10 @@
         <v>20</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>352</v>
+        <v>317</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>354</v>
+        <v>319</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>19</v>
@@ -1924,22 +1797,22 @@
     </row>
     <row r="17" spans="1:7">
       <c r="A17" s="5" t="s">
-        <v>357</v>
+        <v>322</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>356</v>
+        <v>321</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>350</v>
+        <v>315</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>353</v>
+        <v>318</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>355</v>
+        <v>320</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>305</v>
+        <v>270</v>
       </c>
       <c r="G17" s="2" t="s">
         <v>7</v>
@@ -1956,19 +1829,19 @@
     </row>
     <row r="19" spans="1:7">
       <c r="A19" s="5" t="s">
-        <v>359</v>
+        <v>324</v>
       </c>
       <c r="B19" s="5" t="s">
         <v>21</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>362</v>
+        <v>327</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>366</v>
+        <v>331</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>367</v>
+        <v>332</v>
       </c>
       <c r="F19" s="2" t="s">
         <v>21</v>
@@ -1979,22 +1852,22 @@
     </row>
     <row r="20" spans="1:7">
       <c r="A20" s="5" t="s">
-        <v>360</v>
+        <v>325</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>306</v>
+        <v>271</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>363</v>
+        <v>328</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>365</v>
+        <v>330</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>368</v>
+        <v>333</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>306</v>
+        <v>271</v>
       </c>
       <c r="G20" s="5" t="s">
         <v>7</v>
@@ -2002,7 +1875,7 @@
     </row>
     <row r="21" spans="1:7">
       <c r="A21" s="5" t="s">
-        <v>361</v>
+        <v>326</v>
       </c>
       <c r="B21" s="5" t="s">
         <v>22</v>
@@ -2011,10 +1884,10 @@
         <v>23</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>364</v>
+        <v>329</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>369</v>
+        <v>334</v>
       </c>
       <c r="F21" s="2" t="s">
         <v>22</v>
@@ -2031,245 +1904,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F10"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="7"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C2" s="2">
-        <f>LEN(B2)</f>
-        <v>10</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="E2" s="2">
-        <f>LEN(D2)</f>
-        <v>12</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C3" s="2">
-        <f t="shared" ref="C3:E9" si="0">LEN(B3)</f>
-        <v>6</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="E3" s="2">
-        <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C4" s="2">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="E4" s="2">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="C5" s="2">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="E5" s="2">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="C6" s="2">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="E6" s="2">
-        <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C7" s="2">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="E7" s="2">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-      <c r="F7" s="7" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="C8" s="2">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="E8" s="2">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="F8" s="7" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="C9" s="2">
-        <f t="shared" si="0"/>
-        <v>13</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="E9" s="2">
-        <f t="shared" si="0"/>
-        <v>14</v>
-      </c>
-      <c r="F9" s="7" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="B10" t="s">
-        <v>66</v>
-      </c>
-      <c r="C10" s="9">
-        <f>MAX(C2:C9)</f>
-        <v>13</v>
-      </c>
-      <c r="D10" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="E10" s="9">
-        <f>MAX(E2:E9)</f>
-        <v>15</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J93"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A28" workbookViewId="0">
       <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
@@ -2285,217 +1922,217 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" s="4" t="s">
-        <v>67</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" s="4" t="s">
-        <v>68</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" s="4" t="s">
-        <v>69</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="4" t="s">
-        <v>70</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="4" t="s">
-        <v>71</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="4" t="s">
-        <v>72</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="4" t="s">
-        <v>73</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="4" t="s">
-        <v>74</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:10">
       <c r="A9" s="4" t="s">
-        <v>75</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:10">
       <c r="A10" s="4" t="s">
-        <v>76</v>
+        <v>41</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>77</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="4" t="s">
-        <v>78</v>
+        <v>43</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>79</v>
+        <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:10">
       <c r="A12" s="4" t="s">
-        <v>80</v>
+        <v>45</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>81</v>
+        <v>46</v>
       </c>
       <c r="H12" s="3" t="s">
         <v>10</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>82</v>
+        <v>47</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>83</v>
+        <v>48</v>
       </c>
     </row>
     <row r="13" spans="1:10">
       <c r="A13" s="4" t="s">
-        <v>84</v>
+        <v>49</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>85</v>
+        <v>50</v>
       </c>
       <c r="H13" s="3" t="s">
         <v>9</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>86</v>
+        <v>51</v>
       </c>
       <c r="J13" s="3" t="s">
-        <v>87</v>
+        <v>52</v>
       </c>
     </row>
     <row r="14" spans="1:10">
       <c r="A14" s="4" t="s">
-        <v>88</v>
+        <v>53</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>89</v>
+        <v>54</v>
       </c>
       <c r="H14" s="3" t="s">
         <v>8</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>90</v>
+        <v>55</v>
       </c>
       <c r="J14" s="3" t="s">
-        <v>91</v>
+        <v>56</v>
       </c>
     </row>
     <row r="15" spans="1:10">
       <c r="A15" s="4" t="s">
-        <v>92</v>
+        <v>57</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>93</v>
+        <v>58</v>
       </c>
     </row>
     <row r="16" spans="1:10">
       <c r="A16" s="4" t="s">
-        <v>94</v>
+        <v>59</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>95</v>
+        <v>60</v>
       </c>
     </row>
     <row r="17" spans="1:10">
       <c r="A17" s="4" t="s">
-        <v>96</v>
+        <v>61</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>97</v>
+        <v>62</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>98</v>
+        <v>63</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>99</v>
+        <v>64</v>
       </c>
       <c r="J17" s="3" t="s">
-        <v>100</v>
+        <v>65</v>
       </c>
     </row>
     <row r="18" spans="1:10">
       <c r="A18" s="4" t="s">
-        <v>101</v>
+        <v>66</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>102</v>
+        <v>67</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>103</v>
+        <v>68</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>104</v>
+        <v>69</v>
       </c>
       <c r="J18" s="3" t="s">
-        <v>105</v>
+        <v>70</v>
       </c>
     </row>
     <row r="19" spans="1:10">
       <c r="A19" s="4" t="s">
-        <v>106</v>
+        <v>71</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>107</v>
+        <v>72</v>
       </c>
       <c r="H19" s="3" t="s">
         <v>21</v>
       </c>
       <c r="I19" s="3" t="s">
-        <v>108</v>
+        <v>73</v>
       </c>
       <c r="J19" s="3" t="s">
-        <v>109</v>
+        <v>74</v>
       </c>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="4" t="s">
-        <v>110</v>
+        <v>75</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>111</v>
+        <v>76</v>
       </c>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="4" t="s">
-        <v>112</v>
+        <v>77</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>113</v>
+        <v>78</v>
       </c>
       <c r="H21" s="3" t="s">
         <v>11</v>
       </c>
       <c r="I21" s="3" t="s">
-        <v>114</v>
+        <v>79</v>
       </c>
       <c r="J21" s="3" t="s">
-        <v>115</v>
+        <v>80</v>
       </c>
     </row>
     <row r="22" spans="1:10">
       <c r="A22" s="4" t="s">
-        <v>116</v>
+        <v>81</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>117</v>
+        <v>82</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>118</v>
+        <v>83</v>
       </c>
       <c r="I22" s="3" t="s">
         <v>24</v>
@@ -2506,30 +2143,30 @@
     </row>
     <row r="23" spans="1:10">
       <c r="A23" s="4" t="s">
-        <v>119</v>
+        <v>84</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>120</v>
+        <v>85</v>
       </c>
       <c r="H23" s="3" t="s">
         <v>12</v>
       </c>
       <c r="I23" s="3" t="s">
-        <v>121</v>
+        <v>86</v>
       </c>
       <c r="J23" s="3" t="s">
-        <v>122</v>
+        <v>87</v>
       </c>
     </row>
     <row r="24" spans="1:10">
       <c r="A24" s="4" t="s">
-        <v>123</v>
+        <v>88</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>124</v>
+        <v>89</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>125</v>
+        <v>90</v>
       </c>
       <c r="I24" s="3" t="s">
         <v>25</v>
@@ -2540,30 +2177,30 @@
     </row>
     <row r="25" spans="1:10">
       <c r="A25" s="4" t="s">
-        <v>126</v>
+        <v>91</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>127</v>
+        <v>92</v>
       </c>
       <c r="H25" s="3" t="s">
         <v>13</v>
       </c>
       <c r="I25" s="3" t="s">
-        <v>128</v>
+        <v>93</v>
       </c>
       <c r="J25" s="3" t="s">
-        <v>129</v>
+        <v>94</v>
       </c>
     </row>
     <row r="26" spans="1:10">
       <c r="A26" s="4" t="s">
-        <v>130</v>
+        <v>95</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>131</v>
+        <v>96</v>
       </c>
       <c r="H26" s="3" t="s">
-        <v>132</v>
+        <v>97</v>
       </c>
       <c r="I26" s="3" t="s">
         <v>26</v>
@@ -2574,30 +2211,30 @@
     </row>
     <row r="27" spans="1:10">
       <c r="A27" s="4" t="s">
-        <v>133</v>
+        <v>98</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>134</v>
+        <v>99</v>
       </c>
       <c r="H27" s="3" t="s">
         <v>14</v>
       </c>
       <c r="I27" s="3" t="s">
-        <v>135</v>
+        <v>100</v>
       </c>
       <c r="J27" s="3" t="s">
-        <v>136</v>
+        <v>101</v>
       </c>
     </row>
     <row r="28" spans="1:10">
       <c r="A28" s="4" t="s">
-        <v>137</v>
+        <v>102</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>138</v>
+        <v>103</v>
       </c>
       <c r="H28" s="3" t="s">
-        <v>139</v>
+        <v>104</v>
       </c>
       <c r="I28" s="3" t="s">
         <v>27</v>
@@ -2608,465 +2245,465 @@
     </row>
     <row r="29" spans="1:10">
       <c r="A29" s="4" t="s">
-        <v>140</v>
+        <v>105</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>141</v>
+        <v>106</v>
       </c>
       <c r="H29" s="3" t="s">
         <v>15</v>
       </c>
       <c r="I29" s="3" t="s">
-        <v>142</v>
+        <v>107</v>
       </c>
       <c r="J29" s="3" t="s">
-        <v>143</v>
+        <v>108</v>
       </c>
     </row>
     <row r="30" spans="1:10">
       <c r="A30" s="4" t="s">
-        <v>144</v>
+        <v>109</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>145</v>
+        <v>110</v>
       </c>
       <c r="H30" s="3" t="s">
-        <v>146</v>
+        <v>111</v>
       </c>
       <c r="I30" s="3" t="s">
-        <v>147</v>
+        <v>112</v>
       </c>
       <c r="J30" s="3" t="s">
-        <v>148</v>
+        <v>113</v>
       </c>
     </row>
     <row r="31" spans="1:10">
       <c r="A31" s="4" t="s">
-        <v>149</v>
+        <v>114</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>150</v>
+        <v>115</v>
       </c>
       <c r="H31" s="3" t="s">
-        <v>151</v>
+        <v>116</v>
       </c>
       <c r="I31" s="3" t="s">
-        <v>152</v>
+        <v>117</v>
       </c>
       <c r="J31" s="3" t="s">
-        <v>153</v>
+        <v>118</v>
       </c>
     </row>
     <row r="32" spans="1:10">
       <c r="A32" s="4" t="s">
-        <v>154</v>
+        <v>119</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>155</v>
+        <v>120</v>
       </c>
       <c r="H32" s="3" t="s">
-        <v>156</v>
+        <v>121</v>
       </c>
       <c r="I32" s="3" t="s">
-        <v>157</v>
+        <v>122</v>
       </c>
       <c r="J32" s="3" t="s">
-        <v>158</v>
+        <v>123</v>
       </c>
     </row>
     <row r="33" spans="1:10">
       <c r="A33" s="4" t="s">
-        <v>159</v>
+        <v>124</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>160</v>
+        <v>125</v>
       </c>
     </row>
     <row r="34" spans="1:10">
       <c r="A34" s="4" t="s">
-        <v>161</v>
+        <v>126</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>162</v>
+        <v>127</v>
       </c>
     </row>
     <row r="35" spans="1:10">
       <c r="A35" s="4" t="s">
-        <v>163</v>
+        <v>128</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>164</v>
+        <v>129</v>
       </c>
       <c r="H35" s="3" t="s">
         <v>18</v>
       </c>
       <c r="I35" s="3" t="s">
-        <v>165</v>
+        <v>130</v>
       </c>
       <c r="J35" s="3" t="s">
-        <v>166</v>
+        <v>131</v>
       </c>
     </row>
     <row r="36" spans="1:10">
       <c r="A36" s="4" t="s">
-        <v>167</v>
+        <v>132</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>168</v>
+        <v>133</v>
       </c>
       <c r="H36" s="3" t="s">
         <v>17</v>
       </c>
       <c r="I36" s="3" t="s">
-        <v>169</v>
+        <v>134</v>
       </c>
       <c r="J36" s="3" t="s">
-        <v>170</v>
+        <v>135</v>
       </c>
     </row>
     <row r="37" spans="1:10">
       <c r="A37" s="4" t="s">
-        <v>171</v>
+        <v>136</v>
       </c>
       <c r="G37" s="3" t="s">
-        <v>172</v>
+        <v>137</v>
       </c>
     </row>
     <row r="38" spans="1:10">
       <c r="A38" s="4" t="s">
-        <v>173</v>
+        <v>138</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>174</v>
+        <v>139</v>
       </c>
     </row>
     <row r="39" spans="1:10">
       <c r="A39" s="4" t="s">
-        <v>175</v>
+        <v>140</v>
       </c>
       <c r="G39" s="3" t="s">
-        <v>176</v>
+        <v>141</v>
       </c>
     </row>
     <row r="40" spans="1:10">
       <c r="A40" s="4" t="s">
-        <v>177</v>
+        <v>142</v>
       </c>
       <c r="G40" s="3" t="s">
-        <v>178</v>
+        <v>143</v>
       </c>
     </row>
     <row r="41" spans="1:10">
       <c r="A41" s="4" t="s">
-        <v>179</v>
+        <v>144</v>
       </c>
       <c r="G41" s="3" t="s">
-        <v>180</v>
+        <v>145</v>
       </c>
     </row>
     <row r="42" spans="1:10">
       <c r="A42" s="4" t="s">
-        <v>181</v>
+        <v>146</v>
       </c>
       <c r="G42" s="3" t="s">
-        <v>182</v>
+        <v>147</v>
       </c>
     </row>
     <row r="43" spans="1:10">
       <c r="A43" s="4" t="s">
-        <v>183</v>
+        <v>148</v>
       </c>
       <c r="G43" s="3" t="s">
-        <v>184</v>
+        <v>149</v>
       </c>
     </row>
     <row r="44" spans="1:10">
       <c r="A44" s="4" t="s">
-        <v>185</v>
+        <v>150</v>
       </c>
       <c r="G44" s="3" t="s">
-        <v>186</v>
+        <v>151</v>
       </c>
     </row>
     <row r="45" spans="1:10">
       <c r="A45" s="4" t="s">
-        <v>187</v>
+        <v>152</v>
       </c>
       <c r="G45" s="3" t="s">
-        <v>188</v>
+        <v>153</v>
       </c>
       <c r="H45" s="3" t="s">
-        <v>189</v>
+        <v>154</v>
       </c>
       <c r="I45" s="3" t="s">
-        <v>190</v>
+        <v>155</v>
       </c>
       <c r="J45" s="3" t="s">
-        <v>191</v>
+        <v>156</v>
       </c>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="4" t="s">
-        <v>192</v>
+        <v>157</v>
       </c>
       <c r="G46" s="3" t="s">
-        <v>193</v>
+        <v>158</v>
       </c>
       <c r="H46" s="3" t="s">
-        <v>194</v>
+        <v>159</v>
       </c>
       <c r="I46" s="3" t="s">
-        <v>195</v>
+        <v>160</v>
       </c>
       <c r="J46" s="3" t="s">
-        <v>196</v>
+        <v>161</v>
       </c>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="4" t="s">
-        <v>197</v>
+        <v>162</v>
       </c>
       <c r="G47" s="3" t="s">
-        <v>198</v>
+        <v>163</v>
       </c>
       <c r="H47" s="3" t="s">
-        <v>199</v>
+        <v>164</v>
       </c>
       <c r="I47" s="3" t="s">
-        <v>200</v>
+        <v>165</v>
       </c>
       <c r="J47" s="3" t="s">
-        <v>201</v>
+        <v>166</v>
       </c>
     </row>
     <row r="48" spans="1:10">
       <c r="A48" s="4" t="s">
-        <v>202</v>
+        <v>167</v>
       </c>
     </row>
     <row r="49" spans="1:1">
       <c r="A49" s="4" t="s">
-        <v>74</v>
+        <v>39</v>
       </c>
     </row>
     <row r="50" spans="1:1">
       <c r="A50" s="4" t="s">
-        <v>75</v>
+        <v>40</v>
       </c>
     </row>
     <row r="51" spans="1:1">
       <c r="A51" s="4" t="s">
-        <v>203</v>
+        <v>168</v>
       </c>
     </row>
     <row r="52" spans="1:1">
       <c r="A52" s="4" t="s">
-        <v>78</v>
+        <v>43</v>
       </c>
     </row>
     <row r="53" spans="1:1">
       <c r="A53" s="4" t="s">
-        <v>80</v>
+        <v>45</v>
       </c>
     </row>
     <row r="54" spans="1:1">
       <c r="A54" s="4" t="s">
-        <v>84</v>
+        <v>49</v>
       </c>
     </row>
     <row r="55" spans="1:1">
       <c r="A55" s="4" t="s">
-        <v>88</v>
+        <v>53</v>
       </c>
     </row>
     <row r="56" spans="1:1">
       <c r="A56" s="4" t="s">
-        <v>92</v>
+        <v>57</v>
       </c>
     </row>
     <row r="57" spans="1:1">
       <c r="A57" s="4" t="s">
-        <v>94</v>
+        <v>59</v>
       </c>
     </row>
     <row r="58" spans="1:1">
       <c r="A58" s="4" t="s">
-        <v>96</v>
+        <v>61</v>
       </c>
     </row>
     <row r="59" spans="1:1">
       <c r="A59" s="4" t="s">
-        <v>101</v>
+        <v>66</v>
       </c>
     </row>
     <row r="60" spans="1:1">
       <c r="A60" s="4" t="s">
-        <v>106</v>
+        <v>71</v>
       </c>
     </row>
     <row r="61" spans="1:1">
       <c r="A61" s="4" t="s">
-        <v>110</v>
+        <v>75</v>
       </c>
     </row>
     <row r="62" spans="1:1">
       <c r="A62" s="4" t="s">
-        <v>112</v>
+        <v>77</v>
       </c>
     </row>
     <row r="63" spans="1:1">
       <c r="A63" s="4" t="s">
-        <v>204</v>
+        <v>169</v>
       </c>
     </row>
     <row r="64" spans="1:1">
       <c r="A64" s="4" t="s">
-        <v>205</v>
+        <v>170</v>
       </c>
     </row>
     <row r="65" spans="1:1">
       <c r="A65" s="4" t="s">
-        <v>206</v>
+        <v>171</v>
       </c>
     </row>
     <row r="66" spans="1:1">
       <c r="A66" s="4" t="s">
-        <v>207</v>
+        <v>172</v>
       </c>
     </row>
     <row r="67" spans="1:1">
       <c r="A67" s="4" t="s">
-        <v>208</v>
+        <v>173</v>
       </c>
     </row>
     <row r="68" spans="1:1">
       <c r="A68" s="4" t="s">
-        <v>209</v>
+        <v>174</v>
       </c>
     </row>
     <row r="69" spans="1:1">
       <c r="A69" s="4" t="s">
-        <v>210</v>
+        <v>175</v>
       </c>
     </row>
     <row r="70" spans="1:1">
       <c r="A70" s="4" t="s">
-        <v>211</v>
+        <v>176</v>
       </c>
     </row>
     <row r="71" spans="1:1">
       <c r="A71" s="4" t="s">
-        <v>144</v>
+        <v>109</v>
       </c>
     </row>
     <row r="72" spans="1:1">
       <c r="A72" s="4" t="s">
-        <v>212</v>
+        <v>177</v>
       </c>
     </row>
     <row r="73" spans="1:1">
       <c r="A73" s="4" t="s">
-        <v>213</v>
+        <v>178</v>
       </c>
     </row>
     <row r="74" spans="1:1">
       <c r="A74" s="4" t="s">
-        <v>159</v>
+        <v>124</v>
       </c>
     </row>
     <row r="75" spans="1:1">
       <c r="A75" s="4" t="s">
-        <v>161</v>
+        <v>126</v>
       </c>
     </row>
     <row r="76" spans="1:1">
       <c r="A76" s="4" t="s">
-        <v>163</v>
+        <v>128</v>
       </c>
     </row>
     <row r="77" spans="1:1">
       <c r="A77" s="4" t="s">
-        <v>167</v>
+        <v>132</v>
       </c>
     </row>
     <row r="78" spans="1:1">
       <c r="A78" s="4" t="s">
-        <v>171</v>
+        <v>136</v>
       </c>
     </row>
     <row r="79" spans="1:1">
       <c r="A79" s="4" t="s">
-        <v>173</v>
+        <v>138</v>
       </c>
     </row>
     <row r="80" spans="1:1">
       <c r="A80" s="4" t="s">
-        <v>214</v>
+        <v>179</v>
       </c>
     </row>
     <row r="81" spans="1:1">
       <c r="A81" s="4" t="s">
-        <v>177</v>
+        <v>142</v>
       </c>
     </row>
     <row r="82" spans="1:1">
       <c r="A82" s="4" t="s">
-        <v>179</v>
+        <v>144</v>
       </c>
     </row>
     <row r="83" spans="1:1">
       <c r="A83" s="4" t="s">
-        <v>181</v>
+        <v>146</v>
       </c>
     </row>
     <row r="84" spans="1:1">
       <c r="A84" s="4" t="s">
-        <v>183</v>
+        <v>148</v>
       </c>
     </row>
     <row r="85" spans="1:1">
       <c r="A85" s="4" t="s">
-        <v>185</v>
+        <v>150</v>
       </c>
     </row>
     <row r="86" spans="1:1">
       <c r="A86" s="4" t="s">
-        <v>215</v>
+        <v>180</v>
       </c>
     </row>
     <row r="87" spans="1:1">
       <c r="A87" s="4" t="s">
-        <v>216</v>
+        <v>181</v>
       </c>
     </row>
     <row r="88" spans="1:1">
       <c r="A88" s="4" t="s">
-        <v>217</v>
+        <v>182</v>
       </c>
     </row>
     <row r="89" spans="1:1">
       <c r="A89" s="4" t="s">
-        <v>202</v>
+        <v>167</v>
       </c>
     </row>
     <row r="90" spans="1:1">
       <c r="A90" s="4" t="s">
-        <v>218</v>
+        <v>183</v>
       </c>
     </row>
     <row r="91" spans="1:1">
       <c r="A91" s="4" t="s">
-        <v>219</v>
+        <v>184</v>
       </c>
     </row>
     <row r="92" spans="1:1">
       <c r="A92" s="4" t="s">
-        <v>220</v>
+        <v>185</v>
       </c>
     </row>
     <row r="93" spans="1:1">
       <c r="A93" s="4" t="s">
-        <v>221</v>
+        <v>186</v>
       </c>
     </row>
   </sheetData>
@@ -3075,7 +2712,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C41"/>
   <sheetViews>
@@ -3093,344 +2730,344 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>222</v>
+        <v>187</v>
       </c>
       <c r="B1" t="s">
-        <v>223</v>
+        <v>188</v>
       </c>
       <c r="C1" t="s">
-        <v>292</v>
+        <v>257</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>224</v>
+        <v>189</v>
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="10" t="s">
-        <v>225</v>
-      </c>
-      <c r="B4" s="10" t="s">
-        <v>226</v>
+      <c r="A4" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="2" t="s">
-        <v>227</v>
+        <v>192</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>228</v>
+        <v>193</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="2" t="s">
-        <v>145</v>
+        <v>110</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>229</v>
+        <v>194</v>
       </c>
       <c r="C6" t="s">
-        <v>230</v>
+        <v>195</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="2" t="s">
-        <v>150</v>
+        <v>115</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>231</v>
+        <v>196</v>
       </c>
       <c r="C7" t="s">
-        <v>232</v>
+        <v>197</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="2" t="s">
-        <v>155</v>
+        <v>120</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>233</v>
+        <v>198</v>
       </c>
       <c r="C8" t="s">
-        <v>234</v>
+        <v>199</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" t="s">
-        <v>235</v>
+        <v>200</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="2" t="s">
-        <v>236</v>
+        <v>201</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>237</v>
+        <v>202</v>
       </c>
       <c r="C10" t="s">
-        <v>238</v>
+        <v>203</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="2" t="s">
-        <v>239</v>
+        <v>204</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>237</v>
+        <v>202</v>
       </c>
       <c r="C11" t="s">
-        <v>240</v>
+        <v>205</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="2" t="s">
-        <v>241</v>
+        <v>206</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>242</v>
+        <v>207</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="2" t="s">
-        <v>243</v>
+        <v>208</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>242</v>
+        <v>207</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="2" t="s">
-        <v>244</v>
+        <v>209</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>245</v>
+        <v>210</v>
       </c>
       <c r="C14" t="s">
-        <v>246</v>
+        <v>211</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="2" t="s">
-        <v>247</v>
+        <v>212</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>245</v>
+        <v>210</v>
       </c>
       <c r="C15" t="s">
-        <v>248</v>
+        <v>213</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="2" t="s">
-        <v>249</v>
+        <v>214</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>245</v>
+        <v>210</v>
       </c>
       <c r="C16" t="s">
-        <v>250</v>
+        <v>215</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="2" t="s">
-        <v>251</v>
+        <v>216</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>245</v>
+        <v>210</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="2" t="s">
-        <v>252</v>
+        <v>217</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>237</v>
+        <v>202</v>
       </c>
       <c r="C18" t="s">
-        <v>253</v>
+        <v>218</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="2" t="s">
-        <v>254</v>
+        <v>219</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>237</v>
+        <v>202</v>
       </c>
       <c r="C19" t="s">
-        <v>255</v>
+        <v>220</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" s="2" t="s">
-        <v>256</v>
+        <v>221</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>257</v>
+        <v>222</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" s="2" t="s">
-        <v>258</v>
+        <v>223</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>259</v>
+        <v>224</v>
       </c>
       <c r="C21" t="s">
-        <v>260</v>
+        <v>225</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" s="2" t="s">
-        <v>261</v>
+        <v>226</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>262</v>
+        <v>227</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" s="2" t="s">
-        <v>263</v>
+        <v>228</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>264</v>
+        <v>229</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" s="2" t="s">
-        <v>265</v>
+        <v>230</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>264</v>
+        <v>229</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" s="2" t="s">
-        <v>107</v>
+        <v>72</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>266</v>
+        <v>231</v>
       </c>
       <c r="C25" t="s">
-        <v>267</v>
+        <v>232</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" s="2" t="s">
-        <v>160</v>
+        <v>125</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>268</v>
+        <v>233</v>
       </c>
       <c r="C26" t="s">
-        <v>269</v>
+        <v>234</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" s="2" t="s">
-        <v>93</v>
+        <v>58</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>270</v>
+        <v>235</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" s="2" t="s">
-        <v>271</v>
+        <v>236</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>272</v>
+        <v>237</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" s="2" t="s">
-        <v>273</v>
+        <v>238</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>274</v>
+        <v>239</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" s="2" t="s">
-        <v>275</v>
+        <v>240</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>276</v>
+        <v>241</v>
       </c>
     </row>
     <row r="31" spans="1:3">
       <c r="A31" s="2" t="s">
-        <v>178</v>
+        <v>143</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>277</v>
+        <v>242</v>
       </c>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" s="2" t="s">
-        <v>278</v>
+        <v>243</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>279</v>
+        <v>244</v>
       </c>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" s="2" t="s">
-        <v>280</v>
+        <v>245</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>281</v>
+        <v>246</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" s="2" t="s">
-        <v>282</v>
+        <v>247</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>283</v>
+        <v>248</v>
       </c>
     </row>
     <row r="35" spans="1:3">
       <c r="A35" s="2" t="s">
-        <v>284</v>
+        <v>249</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>285</v>
+        <v>250</v>
       </c>
     </row>
     <row r="36" spans="1:3">
       <c r="A36" s="2" t="s">
-        <v>286</v>
+        <v>251</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>287</v>
+        <v>252</v>
       </c>
     </row>
     <row r="37" spans="1:3">
       <c r="A37" s="2" t="s">
-        <v>288</v>
+        <v>253</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>289</v>
+        <v>254</v>
       </c>
     </row>
     <row r="38" spans="1:3">
       <c r="A38" s="2" t="s">
-        <v>111</v>
+        <v>76</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>290</v>
+        <v>255</v>
       </c>
     </row>
     <row r="39" spans="1:3">
       <c r="A39" s="2" t="s">
-        <v>184</v>
+        <v>149</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>291</v>
+        <v>256</v>
       </c>
     </row>
     <row r="40" spans="1:3">

</xml_diff>